<commit_message>
Updated Major Files v3
Updated Major Files v3
</commit_message>
<xml_diff>
--- a/Batch 2018-20/Sem 1/1st Subject.xlsx
+++ b/Batch 2018-20/Sem 1/1st Subject.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Git\SIMSR-Results-Generator\Batch 2018-20\Sem 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818A32AC-DDEE-4AA2-97CE-D10EEA4E1ECB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3A2B0A-D8D1-4857-9552-F8915A997A80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PM" sheetId="1" r:id="rId1"/>
+    <sheet name="1st Subject" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -343,1072 +343,13 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sheet1"/>
+      <sheetName val="Subjects List"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>MMS18-20/1</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>ADEPU CHETAN GANESH ARCHANA</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>MMS18-20/2</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>ADIVAREKAR PRITI GIRIGHAR NAMRATA</v>
-          </cell>
-        </row>
         <row r="4">
-          <cell r="A4" t="str">
-            <v>MMS18-20/3</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>AMBALLA VISHAL MANOHAR BHARATHI</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>MMS18-20/4</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>AMIN MEENAL PRAVIN ANITA</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>MMS18-20/5</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>ARANJO JULIANA MICHAEL LEENA</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>MMS18-20/6</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>BAGUL PRANAV PRAMOD MEENA</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>MMS18-20/7</v>
-          </cell>
-          <cell r="B8" t="str">
-            <v>BAMANE RENUKA UTTAM SUNITA</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>MMS18-20/8</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>BANSODE NAMRATA SUHAS SANGEETA</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>MMS18-20/9</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>BHAJANI DHANASHREE MANOHAR KAVITA</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>MMS18-20/10</v>
-          </cell>
-          <cell r="B11" t="str">
-            <v>BHANGALE BHUPENDRA RAMESH JYOTI</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>MMS18-20/11</v>
-          </cell>
-          <cell r="B12" t="str">
-            <v>BHATKAR ANAGHA ANIL AKSHATA</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>MMS18-20/12</v>
-          </cell>
-          <cell r="B13" t="str">
-            <v>BHOIR PRANAV SURESH SWETA</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>MMS18-20/13</v>
-          </cell>
-          <cell r="B14" t="str">
-            <v>BHOIR VINAYAK CHINTAMAN SHALINI</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>MMS18-20/14</v>
-          </cell>
-          <cell r="B15" t="str">
-            <v>BHOSALE MAYUR PRATAPRAO USHA</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>MMS18-20/15</v>
-          </cell>
-          <cell r="B16" t="str">
-            <v>BIDVI ABOLI AJENDRA NEHA</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>MMS18-20/16</v>
-          </cell>
-          <cell r="B17" t="str">
-            <v>BORKAR DIPESH SHYAM SANGITA</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>MMS18-20/17</v>
-          </cell>
-          <cell r="B18" t="str">
-            <v>CHANDORKAR PRAJAL MADHUKAR VANITA</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>MMS18-20/18</v>
-          </cell>
-          <cell r="B19" t="str">
-            <v>CHAUDHARI TRUPAL JEEVAN SMITA</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>MMS18-20/19</v>
-          </cell>
-          <cell r="B20" t="str">
-            <v>CHAVAN SURAJ SURESH SUREKHA</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>MMS18-20/20</v>
-          </cell>
-          <cell r="B21" t="str">
-            <v>CHAWHAN SAMTA VIJAY SUNITA</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>MMS18-20/21</v>
-          </cell>
-          <cell r="B22" t="str">
-            <v>DESAI SAURABH HARESH HARSHADA</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>MMS18-20/22</v>
-          </cell>
-          <cell r="B23" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>MMS18-20/23</v>
-          </cell>
-          <cell r="B24" t="str">
-            <v xml:space="preserve">PICHAD DESHMUKH GIRIJA HEMANT MOHINI </v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>MMS18-20/24</v>
-          </cell>
-          <cell r="B25" t="str">
-            <v>DHUMAL SAURABH RAMESH RAJASHREE</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>MMS18-20/25</v>
-          </cell>
-          <cell r="B26" t="str">
-            <v>DSOUZA FLOSSIE JOACHIM RITA</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>MMS18-20/26</v>
-          </cell>
-          <cell r="B27" t="str">
-            <v>DYWARSHETTY NEELIMA VENUGOPAL INDUMATI</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>MMS18-20/27</v>
-          </cell>
-          <cell r="B28" t="str">
-            <v>ERANDE TRUPTI UTTAM SUNITA</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>MMS18-20/28</v>
-          </cell>
-          <cell r="B29" t="str">
-            <v>GAMBHIRRAO MANISH HARISHCHANDRA RANJANA</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>MMS18-20/29</v>
-          </cell>
-          <cell r="B30" t="str">
-            <v>GANGANI ANKIT SURESH TEJAL</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>MMS18-20/30</v>
-          </cell>
-          <cell r="B31" t="str">
-            <v>GANGURDE SAKSHI SUDHIR ASHA</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>MMS18-20/31</v>
-          </cell>
-          <cell r="B32" t="str">
-            <v>GHUMARE SANKET RAMESH JAYSHREE</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>MMS18-20/32</v>
-          </cell>
-          <cell r="B33" t="str">
-            <v>GUPTA NITIN RAJESH CHANDRAKALA</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>MMS18-20/33</v>
-          </cell>
-          <cell r="B34" t="str">
-            <v>HANDE RAHUL RANGARAO NALINI</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>MMS18-20/34</v>
-          </cell>
-          <cell r="B35" t="str">
-            <v>HARMALKAR PRATHAMESH SUBHASH SUBHASHINI</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>MMS18-20/35</v>
-          </cell>
-          <cell r="B36" t="str">
-            <v>KADAM AVIRAJ MOHAN MOHINI</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>MMS18-20/36</v>
-          </cell>
-          <cell r="B37" t="str">
-            <v>JADHAV ANKUR SHIVAJI ANAGHA</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>MMS18-20/37</v>
-          </cell>
-          <cell r="B38" t="str">
-            <v>KADAM AKSHAY RAMESH REEMA</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39" t="str">
-            <v>MMS18-20/38</v>
-          </cell>
-          <cell r="B39" t="str">
-            <v>KADAM SHANTANU DILEEP ANITA</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40" t="str">
-            <v>MMS18-20/39</v>
-          </cell>
-          <cell r="B40" t="str">
-            <v>KAMBLE NIKHIL KESHAVRAO SUSHILA</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41" t="str">
-            <v>MMS18-20/40</v>
-          </cell>
-          <cell r="B41" t="str">
-            <v>KAMBLE SIDDHESH RAMESH SUHASINI</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42" t="str">
-            <v>MMS18-20/41</v>
-          </cell>
-          <cell r="B42" t="str">
-            <v>KATARE MAYANK PRAMOD PRANITA</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43" t="str">
-            <v>MMS18-20/42</v>
-          </cell>
-          <cell r="B43" t="str">
-            <v>KHAN SAIF ALI NIZAM BILKIS</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44" t="str">
-            <v>MMS18-20/43</v>
-          </cell>
-          <cell r="B44" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45" t="str">
-            <v>MMS18-20/44</v>
-          </cell>
-          <cell r="B45" t="str">
-            <v>KOLGE VARDA DEEPAK AARTI</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46" t="str">
-            <v>MMS18-20/45</v>
-          </cell>
-          <cell r="B46" t="str">
-            <v>KOLI PRATIK PRABHAKAR NALINI</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47" t="str">
-            <v>MMS18-20/46</v>
-          </cell>
-          <cell r="B47" t="str">
-            <v>KONDEKAR VAIBHAV VIJAY VAISHALI</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48" t="str">
-            <v>MMS18-20/47</v>
-          </cell>
-          <cell r="B48" t="str">
-            <v>KORE PRASHEEL PRASHANT SHEELA</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49" t="str">
-            <v>MMS18-20/48</v>
-          </cell>
-          <cell r="B49" t="str">
-            <v>LATE VISHAL BALASAHEB PRAMILA</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50" t="str">
-            <v>MMS18-20/49</v>
-          </cell>
-          <cell r="B50" t="str">
-            <v xml:space="preserve">LOKE TEJAL JITENDRA GEETA </v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51" t="str">
-            <v>MMS18-20/50</v>
-          </cell>
-          <cell r="B51" t="str">
-            <v>MANDAVKAR CHAITRALI SANJAY SUCHITA</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52" t="str">
-            <v>MMS18-20/51</v>
-          </cell>
-          <cell r="B52" t="str">
-            <v>MARCHANDE SHWETA SHANTARAM SHEETAL</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53" t="str">
-            <v>MMS18-20/52</v>
-          </cell>
-          <cell r="B53" t="str">
-            <v>MHATRE VARAD GURUNATH SUSHMA</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54" t="str">
-            <v>MMS18-20/53</v>
-          </cell>
-          <cell r="B54" t="str">
-            <v>MISHRA RASHMI SHIVKANT PRATIBHA</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55" t="str">
-            <v>MMS18-20/54</v>
-          </cell>
-          <cell r="B55" t="str">
-            <v>NAIR ANAGHA ANANDKUMAR BHANUMATHI</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56" t="str">
-            <v>MMS18-20/55</v>
-          </cell>
-          <cell r="B56" t="str">
-            <v xml:space="preserve">PANCHAL ANIKET AVINASH AARTI </v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57" t="str">
-            <v>MMS18-20/56</v>
-          </cell>
-          <cell r="B57" t="str">
-            <v>SHAIKH SAMEER MOHAMMADHUSSAIN FATIMA</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58" t="str">
-            <v>MMS18-20/57</v>
-          </cell>
-          <cell r="B58" t="str">
-            <v>SHAMBHARKAR PALLAVI JAGDISH MINAKSHI</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59" t="str">
-            <v>MMS18-20/58</v>
-          </cell>
-          <cell r="B59" t="str">
-            <v>SINGH ASHWIN BHAGWANPRASAD SADHANA</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="A60" t="str">
-            <v>MMS18-20/59</v>
-          </cell>
-          <cell r="B60" t="str">
-            <v>WANKHADE NIKHIL MADHUKAR JYOTI</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="A61" t="str">
-            <v>MMS18-20/60</v>
-          </cell>
-          <cell r="B61" t="str">
-            <v>WORLIKAR SIDDHANT PANKAJ VIDYA</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="A62" t="str">
-            <v>MMS18-20/61</v>
-          </cell>
-          <cell r="B62" t="str">
-            <v>AGATE AKASH PRAKASH KIRAN</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="A63" t="str">
-            <v>MMS18-20/62</v>
-          </cell>
-          <cell r="B63" t="str">
-            <v>AVHAD VISHAKHA MILIND RAKHI</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="A64" t="str">
-            <v>MMS18-20/63</v>
-          </cell>
-          <cell r="B64" t="str">
-            <v>CHILE VARAD KISHOR NEHA</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="A65" t="str">
-            <v>MMS18-20/64</v>
-          </cell>
-          <cell r="B65" t="str">
-            <v>DALVI AKASH SHANKAR NIRMALA</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="A66" t="str">
-            <v>MMS18-20/65</v>
-          </cell>
-          <cell r="B66" t="str">
-            <v>DALVI RUTUJA JAGDISH SUPRIYA</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="A67" t="str">
-            <v>MMS18-20/66</v>
-          </cell>
-          <cell r="B67" t="str">
-            <v xml:space="preserve">GANDHI BHAVIK AJAY HARSHA </v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="A68" t="str">
-            <v>MMS18-20/67</v>
-          </cell>
-          <cell r="B68" t="str">
-            <v>GUNDU MEGHNA GUNASHALI SUJATHA</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="A69" t="str">
-            <v>MMS18-20/68</v>
-          </cell>
-          <cell r="B69" t="str">
-            <v>GUPTA AAYUSH NEELKAMAL MANSHA</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="A70" t="str">
-            <v>MMS18-20/69</v>
-          </cell>
-          <cell r="B70" t="str">
-            <v>GUPTA PRAMOD OMPRAKASH RAMAVATI</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="A71" t="str">
-            <v>MMS18-20/70</v>
-          </cell>
-          <cell r="B71" t="str">
-            <v>JADHAV SHWETA NARESH LATA</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="A72" t="str">
-            <v>MMS18-20/71</v>
-          </cell>
-          <cell r="B72" t="str">
-            <v>INGLE ATHARAVA SHASHIKANT SAILEE</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="A73" t="str">
-            <v>MMS18-20/72</v>
-          </cell>
-          <cell r="B73" t="str">
-            <v>KEMPU VIDYA LAXMAN SHANTAMMA</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74" t="str">
-            <v>MMS18-20/73</v>
-          </cell>
-          <cell r="B74" t="str">
-            <v>KHADE VRUSHALEE SUKHADEV RAJASHREE</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="A75" t="str">
-            <v>MMS18-20/74</v>
-          </cell>
-          <cell r="B75" t="str">
-            <v>KUSHWAHA PRAMOD RAMSAKHA ASHA</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="A76" t="str">
-            <v>MMS18-20/75</v>
-          </cell>
-          <cell r="B76" t="str">
-            <v>MAURYA NEHA JAYSHANKAR GEETA</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="A77" t="str">
-            <v>MMS18-20/76</v>
-          </cell>
-          <cell r="B77" t="str">
-            <v>PANCHAL SWAPNIL SATYAWAN MANASI</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78" t="str">
-            <v>MMS18-20/77</v>
-          </cell>
-          <cell r="B78" t="str">
-            <v>PANDYA VANESHA EDWIN SHASHMIRA</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79" t="str">
-            <v>MMS18-20/78</v>
-          </cell>
-          <cell r="B79" t="str">
-            <v xml:space="preserve">PATEKAR RUPESH GANESH MANJULA </v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="A80" t="str">
-            <v>MMS18-20/79</v>
-          </cell>
-          <cell r="B80" t="str">
-            <v>PATEL PRAGNESH KISHORBHAI DAMYANTIBEN</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="A81" t="str">
-            <v>MMS18-20/80</v>
-          </cell>
-          <cell r="B81" t="str">
-            <v>PATIL CHAITALEE NARESH NAMITA</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="A82" t="str">
-            <v>MMS18-20/81</v>
-          </cell>
-          <cell r="B82" t="str">
-            <v>PEDNEKAR MADHUGANDHA DILIP DEEPALI</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="A83" t="str">
-            <v>MMS18-20/82</v>
-          </cell>
-          <cell r="B83" t="str">
-            <v>PHANSE SAILEE VINOD LEELA</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="A84" t="str">
-            <v>MMS18-20/83</v>
-          </cell>
-          <cell r="B84" t="str">
-            <v>PRASAD ROHAN RAJENDRA RAJKUMARI</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="A85" t="str">
-            <v>MMS18-20/84</v>
-          </cell>
-          <cell r="B85" t="str">
-            <v>RAI JAYESH RAVINDRANATH DIVYA</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="A86" t="str">
-            <v>MMS18-20/85</v>
-          </cell>
-          <cell r="B86" t="str">
-            <v>RANE ASHWINI SANTOSH SAVITA</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="A87" t="str">
-            <v>MMS18-20/86</v>
-          </cell>
-          <cell r="B87" t="str">
-            <v>RANE MAYURI SUHAS ARCHANA</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="A88" t="str">
-            <v>MMS18-20/87</v>
-          </cell>
-          <cell r="B88" t="str">
-            <v>RAORANE SAINI SATISH SANCHITA</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="A89" t="str">
-            <v>MMS18-20/88</v>
-          </cell>
-          <cell r="B89" t="str">
-            <v>RATHOD OMKAR PANDIT DEVIKA</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="A90" t="str">
-            <v>MMS18-20/89</v>
-          </cell>
-          <cell r="B90" t="str">
-            <v>SANGLE SINDHANT NAVANATH PRATIBHA</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="A91" t="str">
-            <v>MMS18-20/90</v>
-          </cell>
-          <cell r="B91" t="str">
-            <v>SARMALKAR SANIKA SUNILDATTA MANISHA</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="A92" t="str">
-            <v>MMS18-20/91</v>
-          </cell>
-          <cell r="B92" t="str">
-            <v>SATAM NEHA ANIL ASMITA</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="A93" t="str">
-            <v>MMS18-20/92</v>
-          </cell>
-          <cell r="B93" t="str">
-            <v>SAWANT AVADHUT RAJAN SHRADDHA</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="A94" t="str">
-            <v>MMS18-20/93</v>
-          </cell>
-          <cell r="B94" t="str">
-            <v>SHARMA PALAK PRAHLAD MRIDULA</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="A95" t="str">
-            <v>MMS18-20/94</v>
-          </cell>
-          <cell r="B95" t="str">
-            <v>SHETTY SHIFALI PRASHANT ASHALATA</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="A96" t="str">
-            <v>MMS18-20/95</v>
-          </cell>
-          <cell r="B96" t="str">
-            <v>SHINDE AKSHAY SURENDRA SUPRIYA</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="A97" t="str">
-            <v>MMS18-20/96</v>
-          </cell>
-          <cell r="B97" t="str">
-            <v>SHINDE ASHUTOSH BHASKAR BHAVANA</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="A98" t="str">
-            <v>MMS18-20/97</v>
-          </cell>
-          <cell r="B98" t="str">
-            <v>SHINDE NIKHIL KRISHNAT MANISHA</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99" t="str">
-            <v>MMS18-20/98</v>
-          </cell>
-          <cell r="B99" t="str">
-            <v>SHINDE SAIRAJ VIKAS SHRADHA</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100" t="str">
-            <v>MMS18-20/99</v>
-          </cell>
-          <cell r="B100" t="str">
-            <v>SHINDE SURAJ SHASHIKANT SHOBHA</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="A101" t="str">
-            <v>MMS18-20/100</v>
-          </cell>
-          <cell r="B101" t="str">
-            <v>SHITYALKAR SHUBHAM DHONDIBA SHALAN</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="A102" t="str">
-            <v>MMS18-20/101</v>
-          </cell>
-          <cell r="B102" t="str">
-            <v>SHIVKAR PRIYANKA JANARDHAN REKHA</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="A103" t="str">
-            <v>MMS18-20/102</v>
-          </cell>
-          <cell r="B103" t="str">
-            <v>SHRIGADI ROHIT DHARMENDRA RUPA</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="A104" t="str">
-            <v>MMS18-20/103</v>
-          </cell>
-          <cell r="B104" t="str">
-            <v>SINGH PRATIK SANJAY MEENA</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="A105" t="str">
-            <v>MMS18-20/104</v>
-          </cell>
-          <cell r="B105" t="str">
-            <v>SINGH VARSHA GURUPRASAD VEENA</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="A106" t="str">
-            <v>MMS18-20/105</v>
-          </cell>
-          <cell r="B106" t="str">
-            <v>SOLANKI PRAKASH RAMESH SUREKHA</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="A107" t="str">
-            <v>MMS18-20/106</v>
-          </cell>
-          <cell r="B107" t="str">
-            <v>SURYAVANSHI MAYURI DILIP BHAGIRATHI</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="A108" t="str">
-            <v>MMS18-20/107</v>
-          </cell>
-          <cell r="B108" t="str">
-            <v>SWAMY VIOLET BENEDICT JULIET</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="A109" t="str">
-            <v>MMS18-20/108</v>
-          </cell>
-          <cell r="B109" t="str">
-            <v xml:space="preserve">TAKKE SAIRAJ SURESH SHRUTIKA </v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="A110" t="str">
-            <v>MMS18-20/109</v>
-          </cell>
-          <cell r="B110" t="str">
-            <v>TALELE BHOOMA GHANASHYAM KALPANA</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="A111" t="str">
-            <v>MMS18-20/110</v>
-          </cell>
-          <cell r="B111" t="str">
-            <v>THOOLKAR SAMEER ARVIND KIRAN</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="A112" t="str">
-            <v>MMS18-20/111</v>
-          </cell>
-          <cell r="B112" t="str">
-            <v>TIWARI VIKAS CHINTAMANI SHAILA</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="A113" t="str">
-            <v>MMS18-20/112</v>
-          </cell>
-          <cell r="B113" t="str">
-            <v>TREHAN VILAKSHAN SUMAN NEENA</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="A114" t="str">
-            <v>MMS18-20/113</v>
-          </cell>
-          <cell r="B114" t="str">
-            <v>VHAVALE YOGESH VIJANAND ANITA</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="A115" t="str">
-            <v>MMS18-20/114</v>
-          </cell>
-          <cell r="B115" t="str">
-            <v>VICHARE SAMRUDHI SANJAY VAIBHAVI</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="A116" t="str">
-            <v>MMS18-20/115</v>
-          </cell>
-          <cell r="B116" t="str">
-            <v>WAGHMARE SHEETAL SURYAKANT SUNANDA</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="A117" t="str">
-            <v>MMS18-20/116</v>
-          </cell>
-          <cell r="B117" t="str">
-            <v>WANI SHUBHAM RAJENDRA  JYOTI</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="A118" t="str">
-            <v>MMS18-20/117</v>
-          </cell>
-          <cell r="B118" t="str">
-            <v>YADAV ANKITA OMPRAKASH SHASHANK DEVI</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="A119" t="str">
-            <v>MMS18-20/118</v>
-          </cell>
-          <cell r="B119" t="str">
-            <v>YADAV ANUSH MAHANTA MALTI</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="A120" t="str">
-            <v>MMS18-20/119</v>
-          </cell>
-          <cell r="B120" t="str">
-            <v>YADAV SUMAN RAMJEET SAVITRIDEVI</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="A121" t="str">
-            <v>MMS18-20/120</v>
-          </cell>
-          <cell r="B121" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="A122" t="str">
-            <v>MMS18-20/121</v>
-          </cell>
-          <cell r="B122" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="A123" t="str">
-            <v>MMS18-20/122</v>
-          </cell>
-          <cell r="B123" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="A124" t="str">
-            <v>MMS18-20/123</v>
-          </cell>
-          <cell r="B124" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="A125" t="str">
-            <v>MMS18-20/124</v>
-          </cell>
-          <cell r="B125" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="A126" t="str">
-            <v>MMS18-20/125</v>
-          </cell>
-          <cell r="B126" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="A127" t="str">
-            <v>MMS18-20/126</v>
-          </cell>
-          <cell r="B127" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="A128" t="str">
-            <v>MMS18-20/127</v>
-          </cell>
-          <cell r="B128" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="A129" t="str">
-            <v>MMS18-20/128</v>
-          </cell>
-          <cell r="B129" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="A130" t="str">
-            <v>MMS18-20/129</v>
-          </cell>
-          <cell r="B130" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="A131" t="str">
-            <v>MMS18-20/130</v>
-          </cell>
-          <cell r="B131" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="A132" t="str">
-            <v>MMS18-20/131</v>
-          </cell>
-          <cell r="B132" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="A133" t="str">
-            <v>MMS18-20/132</v>
-          </cell>
-          <cell r="B133" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="A134" t="str">
-            <v>MMS18-20/133</v>
-          </cell>
-          <cell r="B134" t="str">
-            <v>*** (NOT AVAILABLE) ***</v>
+          <cell r="C4" t="str">
+            <v>Perspective Management</v>
           </cell>
         </row>
       </sheetData>
@@ -1421,13 +362,1072 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Subjects List"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>MMS18-20/1</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>ADEPU CHETAN GANESH ARCHANA</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>MMS18-20/2</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>ADIVAREKAR PRITI GIRIGHAR NAMRATA</v>
+          </cell>
+        </row>
         <row r="4">
-          <cell r="C4" t="str">
-            <v>Perspective Management</v>
+          <cell r="A4" t="str">
+            <v>MMS18-20/3</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>AMBALLA VISHAL MANOHAR BHARATHI</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>MMS18-20/4</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>AMIN MEENAL PRAVIN ANITA</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>MMS18-20/5</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>ARANJO JULIANA MICHAEL LEENA</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>MMS18-20/6</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>BAGUL PRANAV PRAMOD MEENA</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>MMS18-20/7</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>BAMANE RENUKA UTTAM SUNITA</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>MMS18-20/8</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>BANSODE NAMRATA SUHAS SANGEETA</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>MMS18-20/9</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>BHAJANI DHANASHREE MANOHAR KAVITA</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>MMS18-20/10</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>BHANGALE BHUPENDRA RAMESH JYOTI</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>MMS18-20/11</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>BHATKAR ANAGHA ANIL AKSHATA</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>MMS18-20/12</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>BHOIR PRANAV SURESH SWETA</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>MMS18-20/13</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>BHOIR VINAYAK CHINTAMAN SHALINI</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>MMS18-20/14</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>BHOSALE MAYUR PRATAPRAO USHA</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>MMS18-20/15</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>BIDVI ABOLI AJENDRA NEHA</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>MMS18-20/16</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>BORKAR DIPESH SHYAM SANGITA</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>MMS18-20/17</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>CHANDORKAR PRAJAL MADHUKAR VANITA</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>MMS18-20/18</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>CHAUDHARI TRUPAL JEEVAN SMITA</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>MMS18-20/19</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>CHAVAN SURAJ SURESH SUREKHA</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>MMS18-20/20</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>CHAWHAN SAMTA VIJAY SUNITA</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>MMS18-20/21</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>DESAI SAURABH HARESH HARSHADA</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>MMS18-20/22</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>MMS18-20/23</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v xml:space="preserve">PICHAD DESHMUKH GIRIJA HEMANT MOHINI </v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>MMS18-20/24</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v>DHUMAL SAURABH RAMESH RAJASHREE</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>MMS18-20/25</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>DSOUZA FLOSSIE JOACHIM RITA</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>MMS18-20/26</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>DYWARSHETTY NEELIMA VENUGOPAL INDUMATI</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>MMS18-20/27</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>ERANDE TRUPTI UTTAM SUNITA</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>MMS18-20/28</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>GAMBHIRRAO MANISH HARISHCHANDRA RANJANA</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>MMS18-20/29</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>GANGANI ANKIT SURESH TEJAL</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>MMS18-20/30</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v>GANGURDE SAKSHI SUDHIR ASHA</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>MMS18-20/31</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>GHUMARE SANKET RAMESH JAYSHREE</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>MMS18-20/32</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>GUPTA NITIN RAJESH CHANDRAKALA</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>MMS18-20/33</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>HANDE RAHUL RANGARAO NALINI</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>MMS18-20/34</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v>HARMALKAR PRATHAMESH SUBHASH SUBHASHINI</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>MMS18-20/35</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v>KADAM AVIRAJ MOHAN MOHINI</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>MMS18-20/36</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v>JADHAV ANKUR SHIVAJI ANAGHA</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>MMS18-20/37</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v>KADAM AKSHAY RAMESH REEMA</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>MMS18-20/38</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v>KADAM SHANTANU DILEEP ANITA</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>MMS18-20/39</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v>KAMBLE NIKHIL KESHAVRAO SUSHILA</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>MMS18-20/40</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>KAMBLE SIDDHESH RAMESH SUHASINI</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>MMS18-20/41</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v>KATARE MAYANK PRAMOD PRANITA</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>MMS18-20/42</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>KHAN SAIF ALI NIZAM BILKIS</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>MMS18-20/43</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>MMS18-20/44</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v>KOLGE VARDA DEEPAK AARTI</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>MMS18-20/45</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>KOLI PRATIK PRABHAKAR NALINI</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>MMS18-20/46</v>
+          </cell>
+          <cell r="B47" t="str">
+            <v>KONDEKAR VAIBHAV VIJAY VAISHALI</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>MMS18-20/47</v>
+          </cell>
+          <cell r="B48" t="str">
+            <v>KORE PRASHEEL PRASHANT SHEELA</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>MMS18-20/48</v>
+          </cell>
+          <cell r="B49" t="str">
+            <v>LATE VISHAL BALASAHEB PRAMILA</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>MMS18-20/49</v>
+          </cell>
+          <cell r="B50" t="str">
+            <v xml:space="preserve">LOKE TEJAL JITENDRA GEETA </v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>MMS18-20/50</v>
+          </cell>
+          <cell r="B51" t="str">
+            <v>MANDAVKAR CHAITRALI SANJAY SUCHITA</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>MMS18-20/51</v>
+          </cell>
+          <cell r="B52" t="str">
+            <v>MARCHANDE SHWETA SHANTARAM SHEETAL</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>MMS18-20/52</v>
+          </cell>
+          <cell r="B53" t="str">
+            <v>MHATRE VARAD GURUNATH SUSHMA</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>MMS18-20/53</v>
+          </cell>
+          <cell r="B54" t="str">
+            <v>MISHRA RASHMI SHIVKANT PRATIBHA</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>MMS18-20/54</v>
+          </cell>
+          <cell r="B55" t="str">
+            <v>NAIR ANAGHA ANANDKUMAR BHANUMATHI</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56" t="str">
+            <v>MMS18-20/55</v>
+          </cell>
+          <cell r="B56" t="str">
+            <v xml:space="preserve">PANCHAL ANIKET AVINASH AARTI </v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57" t="str">
+            <v>MMS18-20/56</v>
+          </cell>
+          <cell r="B57" t="str">
+            <v>SHAIKH SAMEER MOHAMMADHUSSAIN FATIMA</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58" t="str">
+            <v>MMS18-20/57</v>
+          </cell>
+          <cell r="B58" t="str">
+            <v>SHAMBHARKAR PALLAVI JAGDISH MINAKSHI</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v>MMS18-20/58</v>
+          </cell>
+          <cell r="B59" t="str">
+            <v>SINGH ASHWIN BHAGWANPRASAD SADHANA</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60" t="str">
+            <v>MMS18-20/59</v>
+          </cell>
+          <cell r="B60" t="str">
+            <v>WANKHADE NIKHIL MADHUKAR JYOTI</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61" t="str">
+            <v>MMS18-20/60</v>
+          </cell>
+          <cell r="B61" t="str">
+            <v>WORLIKAR SIDDHANT PANKAJ VIDYA</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62" t="str">
+            <v>MMS18-20/61</v>
+          </cell>
+          <cell r="B62" t="str">
+            <v>AGATE AKASH PRAKASH KIRAN</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63" t="str">
+            <v>MMS18-20/62</v>
+          </cell>
+          <cell r="B63" t="str">
+            <v>AVHAD VISHAKHA MILIND RAKHI</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>MMS18-20/63</v>
+          </cell>
+          <cell r="B64" t="str">
+            <v>CHILE VARAD KISHOR NEHA</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65" t="str">
+            <v>MMS18-20/64</v>
+          </cell>
+          <cell r="B65" t="str">
+            <v>DALVI AKASH SHANKAR NIRMALA</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66" t="str">
+            <v>MMS18-20/65</v>
+          </cell>
+          <cell r="B66" t="str">
+            <v>DALVI RUTUJA JAGDISH SUPRIYA</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v>MMS18-20/66</v>
+          </cell>
+          <cell r="B67" t="str">
+            <v xml:space="preserve">GANDHI BHAVIK AJAY HARSHA </v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v>MMS18-20/67</v>
+          </cell>
+          <cell r="B68" t="str">
+            <v>GUNDU MEGHNA GUNASHALI SUJATHA</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69" t="str">
+            <v>MMS18-20/68</v>
+          </cell>
+          <cell r="B69" t="str">
+            <v>GUPTA AAYUSH NEELKAMAL MANSHA</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70" t="str">
+            <v>MMS18-20/69</v>
+          </cell>
+          <cell r="B70" t="str">
+            <v>GUPTA PRAMOD OMPRAKASH RAMAVATI</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71" t="str">
+            <v>MMS18-20/70</v>
+          </cell>
+          <cell r="B71" t="str">
+            <v>JADHAV SHWETA NARESH LATA</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72" t="str">
+            <v>MMS18-20/71</v>
+          </cell>
+          <cell r="B72" t="str">
+            <v>INGLE ATHARAVA SHASHIKANT SAILEE</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73" t="str">
+            <v>MMS18-20/72</v>
+          </cell>
+          <cell r="B73" t="str">
+            <v>KEMPU VIDYA LAXMAN SHANTAMMA</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74" t="str">
+            <v>MMS18-20/73</v>
+          </cell>
+          <cell r="B74" t="str">
+            <v>KHADE VRUSHALEE SUKHADEV RAJASHREE</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75" t="str">
+            <v>MMS18-20/74</v>
+          </cell>
+          <cell r="B75" t="str">
+            <v>KUSHWAHA PRAMOD RAMSAKHA ASHA</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76" t="str">
+            <v>MMS18-20/75</v>
+          </cell>
+          <cell r="B76" t="str">
+            <v>MAURYA NEHA JAYSHANKAR GEETA</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>MMS18-20/76</v>
+          </cell>
+          <cell r="B77" t="str">
+            <v>PANCHAL SWAPNIL SATYAWAN MANASI</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78" t="str">
+            <v>MMS18-20/77</v>
+          </cell>
+          <cell r="B78" t="str">
+            <v>PANDYA VANESHA EDWIN SHASHMIRA</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79" t="str">
+            <v>MMS18-20/78</v>
+          </cell>
+          <cell r="B79" t="str">
+            <v xml:space="preserve">PATEKAR RUPESH GANESH MANJULA </v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80" t="str">
+            <v>MMS18-20/79</v>
+          </cell>
+          <cell r="B80" t="str">
+            <v>PATEL PRAGNESH KISHORBHAI DAMYANTIBEN</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81" t="str">
+            <v>MMS18-20/80</v>
+          </cell>
+          <cell r="B81" t="str">
+            <v>PATIL CHAITALEE NARESH NAMITA</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82" t="str">
+            <v>MMS18-20/81</v>
+          </cell>
+          <cell r="B82" t="str">
+            <v>PEDNEKAR MADHUGANDHA DILIP DEEPALI</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83" t="str">
+            <v>MMS18-20/82</v>
+          </cell>
+          <cell r="B83" t="str">
+            <v>PHANSE SAILEE VINOD LEELA</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84" t="str">
+            <v>MMS18-20/83</v>
+          </cell>
+          <cell r="B84" t="str">
+            <v>PRASAD ROHAN RAJENDRA RAJKUMARI</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85" t="str">
+            <v>MMS18-20/84</v>
+          </cell>
+          <cell r="B85" t="str">
+            <v>RAI JAYESH RAVINDRANATH DIVYA</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86" t="str">
+            <v>MMS18-20/85</v>
+          </cell>
+          <cell r="B86" t="str">
+            <v>RANE ASHWINI SANTOSH SAVITA</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87" t="str">
+            <v>MMS18-20/86</v>
+          </cell>
+          <cell r="B87" t="str">
+            <v>RANE MAYURI SUHAS ARCHANA</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88" t="str">
+            <v>MMS18-20/87</v>
+          </cell>
+          <cell r="B88" t="str">
+            <v>RAORANE SAINI SATISH SANCHITA</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89" t="str">
+            <v>MMS18-20/88</v>
+          </cell>
+          <cell r="B89" t="str">
+            <v>RATHOD OMKAR PANDIT DEVIKA</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90" t="str">
+            <v>MMS18-20/89</v>
+          </cell>
+          <cell r="B90" t="str">
+            <v>SANGLE SINDHANT NAVANATH PRATIBHA</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91" t="str">
+            <v>MMS18-20/90</v>
+          </cell>
+          <cell r="B91" t="str">
+            <v>SARMALKAR SANIKA SUNILDATTA MANISHA</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92" t="str">
+            <v>MMS18-20/91</v>
+          </cell>
+          <cell r="B92" t="str">
+            <v>SATAM NEHA ANIL ASMITA</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93" t="str">
+            <v>MMS18-20/92</v>
+          </cell>
+          <cell r="B93" t="str">
+            <v>SAWANT AVADHUT RAJAN SHRADDHA</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94" t="str">
+            <v>MMS18-20/93</v>
+          </cell>
+          <cell r="B94" t="str">
+            <v>SHARMA PALAK PRAHLAD MRIDULA</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95" t="str">
+            <v>MMS18-20/94</v>
+          </cell>
+          <cell r="B95" t="str">
+            <v>SHETTY SHIFALI PRASHANT ASHALATA</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96" t="str">
+            <v>MMS18-20/95</v>
+          </cell>
+          <cell r="B96" t="str">
+            <v>SHINDE AKSHAY SURENDRA SUPRIYA</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97" t="str">
+            <v>MMS18-20/96</v>
+          </cell>
+          <cell r="B97" t="str">
+            <v>SHINDE ASHUTOSH BHASKAR BHAVANA</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98" t="str">
+            <v>MMS18-20/97</v>
+          </cell>
+          <cell r="B98" t="str">
+            <v>SHINDE NIKHIL KRISHNAT MANISHA</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99" t="str">
+            <v>MMS18-20/98</v>
+          </cell>
+          <cell r="B99" t="str">
+            <v>SHINDE SAIRAJ VIKAS SHRADHA</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100" t="str">
+            <v>MMS18-20/99</v>
+          </cell>
+          <cell r="B100" t="str">
+            <v>SHINDE SURAJ SHASHIKANT SHOBHA</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101" t="str">
+            <v>MMS18-20/100</v>
+          </cell>
+          <cell r="B101" t="str">
+            <v>SHITYALKAR SHUBHAM DHONDIBA SHALAN</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102" t="str">
+            <v>MMS18-20/101</v>
+          </cell>
+          <cell r="B102" t="str">
+            <v>SHIVKAR PRIYANKA JANARDHAN REKHA</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="A103" t="str">
+            <v>MMS18-20/102</v>
+          </cell>
+          <cell r="B103" t="str">
+            <v>SHRIGADI ROHIT DHARMENDRA RUPA</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="A104" t="str">
+            <v>MMS18-20/103</v>
+          </cell>
+          <cell r="B104" t="str">
+            <v>SINGH PRATIK SANJAY MEENA</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="A105" t="str">
+            <v>MMS18-20/104</v>
+          </cell>
+          <cell r="B105" t="str">
+            <v>SINGH VARSHA GURUPRASAD VEENA</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="A106" t="str">
+            <v>MMS18-20/105</v>
+          </cell>
+          <cell r="B106" t="str">
+            <v>SOLANKI PRAKASH RAMESH SUREKHA</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="A107" t="str">
+            <v>MMS18-20/106</v>
+          </cell>
+          <cell r="B107" t="str">
+            <v>SURYAVANSHI MAYURI DILIP BHAGIRATHI</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="A108" t="str">
+            <v>MMS18-20/107</v>
+          </cell>
+          <cell r="B108" t="str">
+            <v>SWAMY VIOLET BENEDICT JULIET</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="A109" t="str">
+            <v>MMS18-20/108</v>
+          </cell>
+          <cell r="B109" t="str">
+            <v xml:space="preserve">TAKKE SAIRAJ SURESH SHRUTIKA </v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="A110" t="str">
+            <v>MMS18-20/109</v>
+          </cell>
+          <cell r="B110" t="str">
+            <v>TALELE BHOOMA GHANASHYAM KALPANA</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="A111" t="str">
+            <v>MMS18-20/110</v>
+          </cell>
+          <cell r="B111" t="str">
+            <v>THOOLKAR SAMEER ARVIND KIRAN</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="A112" t="str">
+            <v>MMS18-20/111</v>
+          </cell>
+          <cell r="B112" t="str">
+            <v>TIWARI VIKAS CHINTAMANI SHAILA</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="A113" t="str">
+            <v>MMS18-20/112</v>
+          </cell>
+          <cell r="B113" t="str">
+            <v>TREHAN VILAKSHAN SUMAN NEENA</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="A114" t="str">
+            <v>MMS18-20/113</v>
+          </cell>
+          <cell r="B114" t="str">
+            <v>VHAVALE YOGESH VIJANAND ANITA</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="A115" t="str">
+            <v>MMS18-20/114</v>
+          </cell>
+          <cell r="B115" t="str">
+            <v>VICHARE SAMRUDHI SANJAY VAIBHAVI</v>
+          </cell>
+        </row>
+        <row r="116">
+          <cell r="A116" t="str">
+            <v>MMS18-20/115</v>
+          </cell>
+          <cell r="B116" t="str">
+            <v>WAGHMARE SHEETAL SURYAKANT SUNANDA</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="A117" t="str">
+            <v>MMS18-20/116</v>
+          </cell>
+          <cell r="B117" t="str">
+            <v>WANI SHUBHAM RAJENDRA  JYOTI</v>
+          </cell>
+        </row>
+        <row r="118">
+          <cell r="A118" t="str">
+            <v>MMS18-20/117</v>
+          </cell>
+          <cell r="B118" t="str">
+            <v>YADAV ANKITA OMPRAKASH SHASHANK DEVI</v>
+          </cell>
+        </row>
+        <row r="119">
+          <cell r="A119" t="str">
+            <v>MMS18-20/118</v>
+          </cell>
+          <cell r="B119" t="str">
+            <v>YADAV ANUSH MAHANTA MALTI</v>
+          </cell>
+        </row>
+        <row r="120">
+          <cell r="A120" t="str">
+            <v>MMS18-20/119</v>
+          </cell>
+          <cell r="B120" t="str">
+            <v>YADAV SUMAN RAMJEET SAVITRIDEVI</v>
+          </cell>
+        </row>
+        <row r="121">
+          <cell r="A121" t="str">
+            <v>MMS18-20/120</v>
+          </cell>
+          <cell r="B121" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="122">
+          <cell r="A122" t="str">
+            <v>MMS18-20/121</v>
+          </cell>
+          <cell r="B122" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="A123" t="str">
+            <v>MMS18-20/122</v>
+          </cell>
+          <cell r="B123" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="A124" t="str">
+            <v>MMS18-20/123</v>
+          </cell>
+          <cell r="B124" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="A125" t="str">
+            <v>MMS18-20/124</v>
+          </cell>
+          <cell r="B125" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="A126" t="str">
+            <v>MMS18-20/125</v>
+          </cell>
+          <cell r="B126" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="A127" t="str">
+            <v>MMS18-20/126</v>
+          </cell>
+          <cell r="B127" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="128">
+          <cell r="A128" t="str">
+            <v>MMS18-20/127</v>
+          </cell>
+          <cell r="B128" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="A129" t="str">
+            <v>MMS18-20/128</v>
+          </cell>
+          <cell r="B129" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="130">
+          <cell r="A130" t="str">
+            <v>MMS18-20/129</v>
+          </cell>
+          <cell r="B130" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="A131" t="str">
+            <v>MMS18-20/130</v>
+          </cell>
+          <cell r="B131" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="A132" t="str">
+            <v>MMS18-20/131</v>
+          </cell>
+          <cell r="B132" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="133">
+          <cell r="A133" t="str">
+            <v>MMS18-20/132</v>
+          </cell>
+          <cell r="B133" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="134">
+          <cell r="A134" t="str">
+            <v>MMS18-20/133</v>
+          </cell>
+          <cell r="B134" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
           </cell>
         </row>
       </sheetData>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="15" t="str">
-        <f>'[2]Subjects List'!$C$4</f>
+        <f>'[1]Subjects List'!$C$4</f>
         <v>Perspective Management</v>
       </c>
       <c r="D1" s="16"/>
@@ -1803,11 +1803,11 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
-        <f>[1]Sheet1!$A2</f>
+        <f>[2]Sheet1!$A2</f>
         <v>MMS18-20/1</v>
       </c>
       <c r="B3" s="12" t="str">
-        <f>[1]Sheet1!$B2</f>
+        <f>[2]Sheet1!$B2</f>
         <v>ADEPU CHETAN GANESH ARCHANA</v>
       </c>
       <c r="C3" s="8">
@@ -1823,11 +1823,11 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="str">
-        <f>[1]Sheet1!$A3</f>
+        <f>[2]Sheet1!$A3</f>
         <v>MMS18-20/2</v>
       </c>
       <c r="B4" s="12" t="str">
-        <f>[1]Sheet1!$B3</f>
+        <f>[2]Sheet1!$B3</f>
         <v>ADIVAREKAR PRITI GIRIGHAR NAMRATA</v>
       </c>
       <c r="C4" s="1">
@@ -1843,11 +1843,11 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
-        <f>[1]Sheet1!$A4</f>
+        <f>[2]Sheet1!$A4</f>
         <v>MMS18-20/3</v>
       </c>
       <c r="B5" s="12" t="str">
-        <f>[1]Sheet1!$B4</f>
+        <f>[2]Sheet1!$B4</f>
         <v>AMBALLA VISHAL MANOHAR BHARATHI</v>
       </c>
       <c r="C5" s="1">
@@ -1863,11 +1863,11 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f>[1]Sheet1!$A5</f>
+        <f>[2]Sheet1!$A5</f>
         <v>MMS18-20/4</v>
       </c>
       <c r="B6" s="12" t="str">
-        <f>[1]Sheet1!$B5</f>
+        <f>[2]Sheet1!$B5</f>
         <v>AMIN MEENAL PRAVIN ANITA</v>
       </c>
       <c r="C6" s="1">
@@ -1883,11 +1883,11 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>[1]Sheet1!$A6</f>
+        <f>[2]Sheet1!$A6</f>
         <v>MMS18-20/5</v>
       </c>
       <c r="B7" s="12" t="str">
-        <f>[1]Sheet1!$B6</f>
+        <f>[2]Sheet1!$B6</f>
         <v>ARANJO JULIANA MICHAEL LEENA</v>
       </c>
       <c r="C7" s="1">
@@ -1903,11 +1903,11 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
-        <f>[1]Sheet1!$A7</f>
+        <f>[2]Sheet1!$A7</f>
         <v>MMS18-20/6</v>
       </c>
       <c r="B8" s="12" t="str">
-        <f>[1]Sheet1!$B7</f>
+        <f>[2]Sheet1!$B7</f>
         <v>BAGUL PRANAV PRAMOD MEENA</v>
       </c>
       <c r="C8" s="1">
@@ -1923,11 +1923,11 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
-        <f>[1]Sheet1!$A8</f>
+        <f>[2]Sheet1!$A8</f>
         <v>MMS18-20/7</v>
       </c>
       <c r="B9" s="12" t="str">
-        <f>[1]Sheet1!$B8</f>
+        <f>[2]Sheet1!$B8</f>
         <v>BAMANE RENUKA UTTAM SUNITA</v>
       </c>
       <c r="C9" s="1">
@@ -1943,11 +1943,11 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
-        <f>[1]Sheet1!$A9</f>
+        <f>[2]Sheet1!$A9</f>
         <v>MMS18-20/8</v>
       </c>
       <c r="B10" s="12" t="str">
-        <f>[1]Sheet1!$B9</f>
+        <f>[2]Sheet1!$B9</f>
         <v>BANSODE NAMRATA SUHAS SANGEETA</v>
       </c>
       <c r="C10" s="1">
@@ -1963,11 +1963,11 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f>[1]Sheet1!$A10</f>
+        <f>[2]Sheet1!$A10</f>
         <v>MMS18-20/9</v>
       </c>
       <c r="B11" s="12" t="str">
-        <f>[1]Sheet1!$B10</f>
+        <f>[2]Sheet1!$B10</f>
         <v>BHAJANI DHANASHREE MANOHAR KAVITA</v>
       </c>
       <c r="C11" s="1">
@@ -1983,11 +1983,11 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
-        <f>[1]Sheet1!$A11</f>
+        <f>[2]Sheet1!$A11</f>
         <v>MMS18-20/10</v>
       </c>
       <c r="B12" s="12" t="str">
-        <f>[1]Sheet1!$B11</f>
+        <f>[2]Sheet1!$B11</f>
         <v>BHANGALE BHUPENDRA RAMESH JYOTI</v>
       </c>
       <c r="C12" s="1">
@@ -2003,11 +2003,11 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
-        <f>[1]Sheet1!$A12</f>
+        <f>[2]Sheet1!$A12</f>
         <v>MMS18-20/11</v>
       </c>
       <c r="B13" s="12" t="str">
-        <f>[1]Sheet1!$B12</f>
+        <f>[2]Sheet1!$B12</f>
         <v>BHATKAR ANAGHA ANIL AKSHATA</v>
       </c>
       <c r="C13" s="1">
@@ -2023,11 +2023,11 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
-        <f>[1]Sheet1!$A13</f>
+        <f>[2]Sheet1!$A13</f>
         <v>MMS18-20/12</v>
       </c>
       <c r="B14" s="12" t="str">
-        <f>[1]Sheet1!$B13</f>
+        <f>[2]Sheet1!$B13</f>
         <v>BHOIR PRANAV SURESH SWETA</v>
       </c>
       <c r="C14" s="1">
@@ -2043,11 +2043,11 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
-        <f>[1]Sheet1!$A14</f>
+        <f>[2]Sheet1!$A14</f>
         <v>MMS18-20/13</v>
       </c>
       <c r="B15" s="12" t="str">
-        <f>[1]Sheet1!$B14</f>
+        <f>[2]Sheet1!$B14</f>
         <v>BHOIR VINAYAK CHINTAMAN SHALINI</v>
       </c>
       <c r="C15" s="1">
@@ -2063,11 +2063,11 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
-        <f>[1]Sheet1!$A15</f>
+        <f>[2]Sheet1!$A15</f>
         <v>MMS18-20/14</v>
       </c>
       <c r="B16" s="12" t="str">
-        <f>[1]Sheet1!$B15</f>
+        <f>[2]Sheet1!$B15</f>
         <v>BHOSALE MAYUR PRATAPRAO USHA</v>
       </c>
       <c r="C16" s="1">
@@ -2083,11 +2083,11 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
-        <f>[1]Sheet1!$A16</f>
+        <f>[2]Sheet1!$A16</f>
         <v>MMS18-20/15</v>
       </c>
       <c r="B17" s="12" t="str">
-        <f>[1]Sheet1!$B16</f>
+        <f>[2]Sheet1!$B16</f>
         <v>BIDVI ABOLI AJENDRA NEHA</v>
       </c>
       <c r="C17" s="1">
@@ -2103,11 +2103,11 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="str">
-        <f>[1]Sheet1!$A17</f>
+        <f>[2]Sheet1!$A17</f>
         <v>MMS18-20/16</v>
       </c>
       <c r="B18" s="12" t="str">
-        <f>[1]Sheet1!$B17</f>
+        <f>[2]Sheet1!$B17</f>
         <v>BORKAR DIPESH SHYAM SANGITA</v>
       </c>
       <c r="C18" s="1">
@@ -2123,11 +2123,11 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="str">
-        <f>[1]Sheet1!$A18</f>
+        <f>[2]Sheet1!$A18</f>
         <v>MMS18-20/17</v>
       </c>
       <c r="B19" s="12" t="str">
-        <f>[1]Sheet1!$B18</f>
+        <f>[2]Sheet1!$B18</f>
         <v>CHANDORKAR PRAJAL MADHUKAR VANITA</v>
       </c>
       <c r="C19" s="1">
@@ -2143,11 +2143,11 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="str">
-        <f>[1]Sheet1!$A19</f>
+        <f>[2]Sheet1!$A19</f>
         <v>MMS18-20/18</v>
       </c>
       <c r="B20" s="12" t="str">
-        <f>[1]Sheet1!$B19</f>
+        <f>[2]Sheet1!$B19</f>
         <v>CHAUDHARI TRUPAL JEEVAN SMITA</v>
       </c>
       <c r="C20" s="1">
@@ -2163,11 +2163,11 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="str">
-        <f>[1]Sheet1!$A20</f>
+        <f>[2]Sheet1!$A20</f>
         <v>MMS18-20/19</v>
       </c>
       <c r="B21" s="12" t="str">
-        <f>[1]Sheet1!$B20</f>
+        <f>[2]Sheet1!$B20</f>
         <v>CHAVAN SURAJ SURESH SUREKHA</v>
       </c>
       <c r="C21" s="1">
@@ -2183,11 +2183,11 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="str">
-        <f>[1]Sheet1!$A21</f>
+        <f>[2]Sheet1!$A21</f>
         <v>MMS18-20/20</v>
       </c>
       <c r="B22" s="12" t="str">
-        <f>[1]Sheet1!$B21</f>
+        <f>[2]Sheet1!$B21</f>
         <v>CHAWHAN SAMTA VIJAY SUNITA</v>
       </c>
       <c r="C22" s="1">
@@ -2203,11 +2203,11 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="str">
-        <f>[1]Sheet1!$A22</f>
+        <f>[2]Sheet1!$A22</f>
         <v>MMS18-20/21</v>
       </c>
       <c r="B23" s="12" t="str">
-        <f>[1]Sheet1!$B22</f>
+        <f>[2]Sheet1!$B22</f>
         <v>DESAI SAURABH HARESH HARSHADA</v>
       </c>
       <c r="C23" s="1">
@@ -2223,11 +2223,11 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="str">
-        <f>[1]Sheet1!$A23</f>
+        <f>[2]Sheet1!$A23</f>
         <v>MMS18-20/22</v>
       </c>
       <c r="B24" s="12" t="str">
-        <f>[1]Sheet1!$B23</f>
+        <f>[2]Sheet1!$B23</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C24" s="1">
@@ -2243,11 +2243,11 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="str">
-        <f>[1]Sheet1!$A24</f>
+        <f>[2]Sheet1!$A24</f>
         <v>MMS18-20/23</v>
       </c>
       <c r="B25" s="12" t="str">
-        <f>[1]Sheet1!$B24</f>
+        <f>[2]Sheet1!$B24</f>
         <v xml:space="preserve">PICHAD DESHMUKH GIRIJA HEMANT MOHINI </v>
       </c>
       <c r="C25" s="1">
@@ -2263,11 +2263,11 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="str">
-        <f>[1]Sheet1!$A25</f>
+        <f>[2]Sheet1!$A25</f>
         <v>MMS18-20/24</v>
       </c>
       <c r="B26" s="12" t="str">
-        <f>[1]Sheet1!$B25</f>
+        <f>[2]Sheet1!$B25</f>
         <v>DHUMAL SAURABH RAMESH RAJASHREE</v>
       </c>
       <c r="C26" s="1">
@@ -2283,11 +2283,11 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="str">
-        <f>[1]Sheet1!$A26</f>
+        <f>[2]Sheet1!$A26</f>
         <v>MMS18-20/25</v>
       </c>
       <c r="B27" s="12" t="str">
-        <f>[1]Sheet1!$B26</f>
+        <f>[2]Sheet1!$B26</f>
         <v>DSOUZA FLOSSIE JOACHIM RITA</v>
       </c>
       <c r="C27" s="1">
@@ -2303,11 +2303,11 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="str">
-        <f>[1]Sheet1!$A27</f>
+        <f>[2]Sheet1!$A27</f>
         <v>MMS18-20/26</v>
       </c>
       <c r="B28" s="12" t="str">
-        <f>[1]Sheet1!$B27</f>
+        <f>[2]Sheet1!$B27</f>
         <v>DYWARSHETTY NEELIMA VENUGOPAL INDUMATI</v>
       </c>
       <c r="C28" s="1">
@@ -2323,11 +2323,11 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="str">
-        <f>[1]Sheet1!$A28</f>
+        <f>[2]Sheet1!$A28</f>
         <v>MMS18-20/27</v>
       </c>
       <c r="B29" s="12" t="str">
-        <f>[1]Sheet1!$B28</f>
+        <f>[2]Sheet1!$B28</f>
         <v>ERANDE TRUPTI UTTAM SUNITA</v>
       </c>
       <c r="C29" s="1">
@@ -2343,11 +2343,11 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="str">
-        <f>[1]Sheet1!$A29</f>
+        <f>[2]Sheet1!$A29</f>
         <v>MMS18-20/28</v>
       </c>
       <c r="B30" s="12" t="str">
-        <f>[1]Sheet1!$B29</f>
+        <f>[2]Sheet1!$B29</f>
         <v>GAMBHIRRAO MANISH HARISHCHANDRA RANJANA</v>
       </c>
       <c r="C30" s="1">
@@ -2363,11 +2363,11 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="str">
-        <f>[1]Sheet1!$A30</f>
+        <f>[2]Sheet1!$A30</f>
         <v>MMS18-20/29</v>
       </c>
       <c r="B31" s="12" t="str">
-        <f>[1]Sheet1!$B30</f>
+        <f>[2]Sheet1!$B30</f>
         <v>GANGANI ANKIT SURESH TEJAL</v>
       </c>
       <c r="C31" s="1">
@@ -2383,11 +2383,11 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="str">
-        <f>[1]Sheet1!$A31</f>
+        <f>[2]Sheet1!$A31</f>
         <v>MMS18-20/30</v>
       </c>
       <c r="B32" s="12" t="str">
-        <f>[1]Sheet1!$B31</f>
+        <f>[2]Sheet1!$B31</f>
         <v>GANGURDE SAKSHI SUDHIR ASHA</v>
       </c>
       <c r="C32" s="1">
@@ -2403,11 +2403,11 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="str">
-        <f>[1]Sheet1!$A32</f>
+        <f>[2]Sheet1!$A32</f>
         <v>MMS18-20/31</v>
       </c>
       <c r="B33" s="12" t="str">
-        <f>[1]Sheet1!$B32</f>
+        <f>[2]Sheet1!$B32</f>
         <v>GHUMARE SANKET RAMESH JAYSHREE</v>
       </c>
       <c r="C33" s="1">
@@ -2423,11 +2423,11 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="str">
-        <f>[1]Sheet1!$A33</f>
+        <f>[2]Sheet1!$A33</f>
         <v>MMS18-20/32</v>
       </c>
       <c r="B34" s="12" t="str">
-        <f>[1]Sheet1!$B33</f>
+        <f>[2]Sheet1!$B33</f>
         <v>GUPTA NITIN RAJESH CHANDRAKALA</v>
       </c>
       <c r="C34" s="1">
@@ -2443,11 +2443,11 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="str">
-        <f>[1]Sheet1!$A34</f>
+        <f>[2]Sheet1!$A34</f>
         <v>MMS18-20/33</v>
       </c>
       <c r="B35" s="12" t="str">
-        <f>[1]Sheet1!$B34</f>
+        <f>[2]Sheet1!$B34</f>
         <v>HANDE RAHUL RANGARAO NALINI</v>
       </c>
       <c r="C35" s="1">
@@ -2463,11 +2463,11 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="str">
-        <f>[1]Sheet1!$A35</f>
+        <f>[2]Sheet1!$A35</f>
         <v>MMS18-20/34</v>
       </c>
       <c r="B36" s="12" t="str">
-        <f>[1]Sheet1!$B35</f>
+        <f>[2]Sheet1!$B35</f>
         <v>HARMALKAR PRATHAMESH SUBHASH SUBHASHINI</v>
       </c>
       <c r="C36" s="1">
@@ -2483,11 +2483,11 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="str">
-        <f>[1]Sheet1!$A36</f>
+        <f>[2]Sheet1!$A36</f>
         <v>MMS18-20/35</v>
       </c>
       <c r="B37" s="12" t="str">
-        <f>[1]Sheet1!$B36</f>
+        <f>[2]Sheet1!$B36</f>
         <v>KADAM AVIRAJ MOHAN MOHINI</v>
       </c>
       <c r="C37" s="1">
@@ -2503,11 +2503,11 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="str">
-        <f>[1]Sheet1!$A37</f>
+        <f>[2]Sheet1!$A37</f>
         <v>MMS18-20/36</v>
       </c>
       <c r="B38" s="12" t="str">
-        <f>[1]Sheet1!$B37</f>
+        <f>[2]Sheet1!$B37</f>
         <v>JADHAV ANKUR SHIVAJI ANAGHA</v>
       </c>
       <c r="C38" s="1">
@@ -2523,11 +2523,11 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="str">
-        <f>[1]Sheet1!$A38</f>
+        <f>[2]Sheet1!$A38</f>
         <v>MMS18-20/37</v>
       </c>
       <c r="B39" s="12" t="str">
-        <f>[1]Sheet1!$B38</f>
+        <f>[2]Sheet1!$B38</f>
         <v>KADAM AKSHAY RAMESH REEMA</v>
       </c>
       <c r="C39" s="1">
@@ -2543,11 +2543,11 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="str">
-        <f>[1]Sheet1!$A39</f>
+        <f>[2]Sheet1!$A39</f>
         <v>MMS18-20/38</v>
       </c>
       <c r="B40" s="12" t="str">
-        <f>[1]Sheet1!$B39</f>
+        <f>[2]Sheet1!$B39</f>
         <v>KADAM SHANTANU DILEEP ANITA</v>
       </c>
       <c r="C40" s="1">
@@ -2563,11 +2563,11 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="str">
-        <f>[1]Sheet1!$A40</f>
+        <f>[2]Sheet1!$A40</f>
         <v>MMS18-20/39</v>
       </c>
       <c r="B41" s="12" t="str">
-        <f>[1]Sheet1!$B40</f>
+        <f>[2]Sheet1!$B40</f>
         <v>KAMBLE NIKHIL KESHAVRAO SUSHILA</v>
       </c>
       <c r="C41" s="1">
@@ -2583,11 +2583,11 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="str">
-        <f>[1]Sheet1!$A41</f>
+        <f>[2]Sheet1!$A41</f>
         <v>MMS18-20/40</v>
       </c>
       <c r="B42" s="12" t="str">
-        <f>[1]Sheet1!$B41</f>
+        <f>[2]Sheet1!$B41</f>
         <v>KAMBLE SIDDHESH RAMESH SUHASINI</v>
       </c>
       <c r="C42" s="1">
@@ -2603,11 +2603,11 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="str">
-        <f>[1]Sheet1!$A42</f>
+        <f>[2]Sheet1!$A42</f>
         <v>MMS18-20/41</v>
       </c>
       <c r="B43" s="12" t="str">
-        <f>[1]Sheet1!$B42</f>
+        <f>[2]Sheet1!$B42</f>
         <v>KATARE MAYANK PRAMOD PRANITA</v>
       </c>
       <c r="C43" s="1">
@@ -2623,11 +2623,11 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="str">
-        <f>[1]Sheet1!$A43</f>
+        <f>[2]Sheet1!$A43</f>
         <v>MMS18-20/42</v>
       </c>
       <c r="B44" s="12" t="str">
-        <f>[1]Sheet1!$B43</f>
+        <f>[2]Sheet1!$B43</f>
         <v>KHAN SAIF ALI NIZAM BILKIS</v>
       </c>
       <c r="C44" s="1">
@@ -2643,11 +2643,11 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="str">
-        <f>[1]Sheet1!$A44</f>
+        <f>[2]Sheet1!$A44</f>
         <v>MMS18-20/43</v>
       </c>
       <c r="B45" s="12" t="str">
-        <f>[1]Sheet1!$B44</f>
+        <f>[2]Sheet1!$B44</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C45" s="1">
@@ -2663,11 +2663,11 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="str">
-        <f>[1]Sheet1!$A45</f>
+        <f>[2]Sheet1!$A45</f>
         <v>MMS18-20/44</v>
       </c>
       <c r="B46" s="12" t="str">
-        <f>[1]Sheet1!$B45</f>
+        <f>[2]Sheet1!$B45</f>
         <v>KOLGE VARDA DEEPAK AARTI</v>
       </c>
       <c r="C46" s="1">
@@ -2683,11 +2683,11 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="str">
-        <f>[1]Sheet1!$A46</f>
+        <f>[2]Sheet1!$A46</f>
         <v>MMS18-20/45</v>
       </c>
       <c r="B47" s="12" t="str">
-        <f>[1]Sheet1!$B46</f>
+        <f>[2]Sheet1!$B46</f>
         <v>KOLI PRATIK PRABHAKAR NALINI</v>
       </c>
       <c r="C47" s="1">
@@ -2703,11 +2703,11 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="str">
-        <f>[1]Sheet1!$A47</f>
+        <f>[2]Sheet1!$A47</f>
         <v>MMS18-20/46</v>
       </c>
       <c r="B48" s="12" t="str">
-        <f>[1]Sheet1!$B47</f>
+        <f>[2]Sheet1!$B47</f>
         <v>KONDEKAR VAIBHAV VIJAY VAISHALI</v>
       </c>
       <c r="C48" s="1">
@@ -2723,11 +2723,11 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="str">
-        <f>[1]Sheet1!$A48</f>
+        <f>[2]Sheet1!$A48</f>
         <v>MMS18-20/47</v>
       </c>
       <c r="B49" s="12" t="str">
-        <f>[1]Sheet1!$B48</f>
+        <f>[2]Sheet1!$B48</f>
         <v>KORE PRASHEEL PRASHANT SHEELA</v>
       </c>
       <c r="C49" s="1">
@@ -2743,11 +2743,11 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="str">
-        <f>[1]Sheet1!$A49</f>
+        <f>[2]Sheet1!$A49</f>
         <v>MMS18-20/48</v>
       </c>
       <c r="B50" s="12" t="str">
-        <f>[1]Sheet1!$B49</f>
+        <f>[2]Sheet1!$B49</f>
         <v>LATE VISHAL BALASAHEB PRAMILA</v>
       </c>
       <c r="C50" s="1">
@@ -2763,11 +2763,11 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="str">
-        <f>[1]Sheet1!$A50</f>
+        <f>[2]Sheet1!$A50</f>
         <v>MMS18-20/49</v>
       </c>
       <c r="B51" s="12" t="str">
-        <f>[1]Sheet1!$B50</f>
+        <f>[2]Sheet1!$B50</f>
         <v xml:space="preserve">LOKE TEJAL JITENDRA GEETA </v>
       </c>
       <c r="C51" s="1">
@@ -2783,11 +2783,11 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="str">
-        <f>[1]Sheet1!$A51</f>
+        <f>[2]Sheet1!$A51</f>
         <v>MMS18-20/50</v>
       </c>
       <c r="B52" s="12" t="str">
-        <f>[1]Sheet1!$B51</f>
+        <f>[2]Sheet1!$B51</f>
         <v>MANDAVKAR CHAITRALI SANJAY SUCHITA</v>
       </c>
       <c r="C52" s="1">
@@ -2803,11 +2803,11 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="str">
-        <f>[1]Sheet1!$A52</f>
+        <f>[2]Sheet1!$A52</f>
         <v>MMS18-20/51</v>
       </c>
       <c r="B53" s="12" t="str">
-        <f>[1]Sheet1!$B52</f>
+        <f>[2]Sheet1!$B52</f>
         <v>MARCHANDE SHWETA SHANTARAM SHEETAL</v>
       </c>
       <c r="C53" s="1">
@@ -2823,11 +2823,11 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="str">
-        <f>[1]Sheet1!$A53</f>
+        <f>[2]Sheet1!$A53</f>
         <v>MMS18-20/52</v>
       </c>
       <c r="B54" s="12" t="str">
-        <f>[1]Sheet1!$B53</f>
+        <f>[2]Sheet1!$B53</f>
         <v>MHATRE VARAD GURUNATH SUSHMA</v>
       </c>
       <c r="C54" s="1">
@@ -2843,11 +2843,11 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="str">
-        <f>[1]Sheet1!$A54</f>
+        <f>[2]Sheet1!$A54</f>
         <v>MMS18-20/53</v>
       </c>
       <c r="B55" s="12" t="str">
-        <f>[1]Sheet1!$B54</f>
+        <f>[2]Sheet1!$B54</f>
         <v>MISHRA RASHMI SHIVKANT PRATIBHA</v>
       </c>
       <c r="C55" s="1">
@@ -2863,11 +2863,11 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="str">
-        <f>[1]Sheet1!$A55</f>
+        <f>[2]Sheet1!$A55</f>
         <v>MMS18-20/54</v>
       </c>
       <c r="B56" s="12" t="str">
-        <f>[1]Sheet1!$B55</f>
+        <f>[2]Sheet1!$B55</f>
         <v>NAIR ANAGHA ANANDKUMAR BHANUMATHI</v>
       </c>
       <c r="C56" s="1">
@@ -2883,11 +2883,11 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="str">
-        <f>[1]Sheet1!$A56</f>
+        <f>[2]Sheet1!$A56</f>
         <v>MMS18-20/55</v>
       </c>
       <c r="B57" s="12" t="str">
-        <f>[1]Sheet1!$B56</f>
+        <f>[2]Sheet1!$B56</f>
         <v xml:space="preserve">PANCHAL ANIKET AVINASH AARTI </v>
       </c>
       <c r="C57" s="1">
@@ -2903,11 +2903,11 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="str">
-        <f>[1]Sheet1!$A57</f>
+        <f>[2]Sheet1!$A57</f>
         <v>MMS18-20/56</v>
       </c>
       <c r="B58" s="12" t="str">
-        <f>[1]Sheet1!$B57</f>
+        <f>[2]Sheet1!$B57</f>
         <v>SHAIKH SAMEER MOHAMMADHUSSAIN FATIMA</v>
       </c>
       <c r="C58" s="1">
@@ -2923,11 +2923,11 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="str">
-        <f>[1]Sheet1!$A58</f>
+        <f>[2]Sheet1!$A58</f>
         <v>MMS18-20/57</v>
       </c>
       <c r="B59" s="12" t="str">
-        <f>[1]Sheet1!$B58</f>
+        <f>[2]Sheet1!$B58</f>
         <v>SHAMBHARKAR PALLAVI JAGDISH MINAKSHI</v>
       </c>
       <c r="C59" s="1">
@@ -2943,11 +2943,11 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="str">
-        <f>[1]Sheet1!$A59</f>
+        <f>[2]Sheet1!$A59</f>
         <v>MMS18-20/58</v>
       </c>
       <c r="B60" s="12" t="str">
-        <f>[1]Sheet1!$B59</f>
+        <f>[2]Sheet1!$B59</f>
         <v>SINGH ASHWIN BHAGWANPRASAD SADHANA</v>
       </c>
       <c r="C60" s="1">
@@ -2963,11 +2963,11 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="str">
-        <f>[1]Sheet1!$A60</f>
+        <f>[2]Sheet1!$A60</f>
         <v>MMS18-20/59</v>
       </c>
       <c r="B61" s="12" t="str">
-        <f>[1]Sheet1!$B60</f>
+        <f>[2]Sheet1!$B60</f>
         <v>WANKHADE NIKHIL MADHUKAR JYOTI</v>
       </c>
       <c r="C61" s="1">
@@ -2983,11 +2983,11 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="str">
-        <f>[1]Sheet1!$A61</f>
+        <f>[2]Sheet1!$A61</f>
         <v>MMS18-20/60</v>
       </c>
       <c r="B62" s="12" t="str">
-        <f>[1]Sheet1!$B61</f>
+        <f>[2]Sheet1!$B61</f>
         <v>WORLIKAR SIDDHANT PANKAJ VIDYA</v>
       </c>
       <c r="C62" s="1">
@@ -3003,11 +3003,11 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="str">
-        <f>[1]Sheet1!$A62</f>
+        <f>[2]Sheet1!$A62</f>
         <v>MMS18-20/61</v>
       </c>
       <c r="B63" s="12" t="str">
-        <f>[1]Sheet1!$B62</f>
+        <f>[2]Sheet1!$B62</f>
         <v>AGATE AKASH PRAKASH KIRAN</v>
       </c>
       <c r="C63" s="1">
@@ -3023,11 +3023,11 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="str">
-        <f>[1]Sheet1!$A63</f>
+        <f>[2]Sheet1!$A63</f>
         <v>MMS18-20/62</v>
       </c>
       <c r="B64" s="12" t="str">
-        <f>[1]Sheet1!$B63</f>
+        <f>[2]Sheet1!$B63</f>
         <v>AVHAD VISHAKHA MILIND RAKHI</v>
       </c>
       <c r="C64" s="1">
@@ -3043,11 +3043,11 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="str">
-        <f>[1]Sheet1!$A64</f>
+        <f>[2]Sheet1!$A64</f>
         <v>MMS18-20/63</v>
       </c>
       <c r="B65" s="12" t="str">
-        <f>[1]Sheet1!$B64</f>
+        <f>[2]Sheet1!$B64</f>
         <v>CHILE VARAD KISHOR NEHA</v>
       </c>
       <c r="C65" s="1">
@@ -3063,11 +3063,11 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="str">
-        <f>[1]Sheet1!$A65</f>
+        <f>[2]Sheet1!$A65</f>
         <v>MMS18-20/64</v>
       </c>
       <c r="B66" s="12" t="str">
-        <f>[1]Sheet1!$B65</f>
+        <f>[2]Sheet1!$B65</f>
         <v>DALVI AKASH SHANKAR NIRMALA</v>
       </c>
       <c r="C66" s="1">
@@ -3083,11 +3083,11 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="str">
-        <f>[1]Sheet1!$A66</f>
+        <f>[2]Sheet1!$A66</f>
         <v>MMS18-20/65</v>
       </c>
       <c r="B67" s="12" t="str">
-        <f>[1]Sheet1!$B66</f>
+        <f>[2]Sheet1!$B66</f>
         <v>DALVI RUTUJA JAGDISH SUPRIYA</v>
       </c>
       <c r="C67" s="1">
@@ -3103,11 +3103,11 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="str">
-        <f>[1]Sheet1!$A67</f>
+        <f>[2]Sheet1!$A67</f>
         <v>MMS18-20/66</v>
       </c>
       <c r="B68" s="12" t="str">
-        <f>[1]Sheet1!$B67</f>
+        <f>[2]Sheet1!$B67</f>
         <v xml:space="preserve">GANDHI BHAVIK AJAY HARSHA </v>
       </c>
       <c r="C68" s="1">
@@ -3123,11 +3123,11 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="str">
-        <f>[1]Sheet1!$A68</f>
+        <f>[2]Sheet1!$A68</f>
         <v>MMS18-20/67</v>
       </c>
       <c r="B69" s="12" t="str">
-        <f>[1]Sheet1!$B68</f>
+        <f>[2]Sheet1!$B68</f>
         <v>GUNDU MEGHNA GUNASHALI SUJATHA</v>
       </c>
       <c r="C69" s="1">
@@ -3143,11 +3143,11 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="str">
-        <f>[1]Sheet1!$A69</f>
+        <f>[2]Sheet1!$A69</f>
         <v>MMS18-20/68</v>
       </c>
       <c r="B70" s="12" t="str">
-        <f>[1]Sheet1!$B69</f>
+        <f>[2]Sheet1!$B69</f>
         <v>GUPTA AAYUSH NEELKAMAL MANSHA</v>
       </c>
       <c r="C70" s="1">
@@ -3163,11 +3163,11 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="str">
-        <f>[1]Sheet1!$A70</f>
+        <f>[2]Sheet1!$A70</f>
         <v>MMS18-20/69</v>
       </c>
       <c r="B71" s="12" t="str">
-        <f>[1]Sheet1!$B70</f>
+        <f>[2]Sheet1!$B70</f>
         <v>GUPTA PRAMOD OMPRAKASH RAMAVATI</v>
       </c>
       <c r="C71" s="1">
@@ -3183,11 +3183,11 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="str">
-        <f>[1]Sheet1!$A71</f>
+        <f>[2]Sheet1!$A71</f>
         <v>MMS18-20/70</v>
       </c>
       <c r="B72" s="12" t="str">
-        <f>[1]Sheet1!$B71</f>
+        <f>[2]Sheet1!$B71</f>
         <v>JADHAV SHWETA NARESH LATA</v>
       </c>
       <c r="C72" s="1">
@@ -3203,11 +3203,11 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="str">
-        <f>[1]Sheet1!$A72</f>
+        <f>[2]Sheet1!$A72</f>
         <v>MMS18-20/71</v>
       </c>
       <c r="B73" s="12" t="str">
-        <f>[1]Sheet1!$B72</f>
+        <f>[2]Sheet1!$B72</f>
         <v>INGLE ATHARAVA SHASHIKANT SAILEE</v>
       </c>
       <c r="C73" s="1">
@@ -3223,11 +3223,11 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="str">
-        <f>[1]Sheet1!$A73</f>
+        <f>[2]Sheet1!$A73</f>
         <v>MMS18-20/72</v>
       </c>
       <c r="B74" s="12" t="str">
-        <f>[1]Sheet1!$B73</f>
+        <f>[2]Sheet1!$B73</f>
         <v>KEMPU VIDYA LAXMAN SHANTAMMA</v>
       </c>
       <c r="C74" s="1">
@@ -3243,11 +3243,11 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="str">
-        <f>[1]Sheet1!$A74</f>
+        <f>[2]Sheet1!$A74</f>
         <v>MMS18-20/73</v>
       </c>
       <c r="B75" s="12" t="str">
-        <f>[1]Sheet1!$B74</f>
+        <f>[2]Sheet1!$B74</f>
         <v>KHADE VRUSHALEE SUKHADEV RAJASHREE</v>
       </c>
       <c r="C75" s="1">
@@ -3263,11 +3263,11 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="str">
-        <f>[1]Sheet1!$A75</f>
+        <f>[2]Sheet1!$A75</f>
         <v>MMS18-20/74</v>
       </c>
       <c r="B76" s="12" t="str">
-        <f>[1]Sheet1!$B75</f>
+        <f>[2]Sheet1!$B75</f>
         <v>KUSHWAHA PRAMOD RAMSAKHA ASHA</v>
       </c>
       <c r="C76" s="1">
@@ -3283,11 +3283,11 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="str">
-        <f>[1]Sheet1!$A76</f>
+        <f>[2]Sheet1!$A76</f>
         <v>MMS18-20/75</v>
       </c>
       <c r="B77" s="12" t="str">
-        <f>[1]Sheet1!$B76</f>
+        <f>[2]Sheet1!$B76</f>
         <v>MAURYA NEHA JAYSHANKAR GEETA</v>
       </c>
       <c r="C77" s="1">
@@ -3303,11 +3303,11 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="str">
-        <f>[1]Sheet1!$A77</f>
+        <f>[2]Sheet1!$A77</f>
         <v>MMS18-20/76</v>
       </c>
       <c r="B78" s="12" t="str">
-        <f>[1]Sheet1!$B77</f>
+        <f>[2]Sheet1!$B77</f>
         <v>PANCHAL SWAPNIL SATYAWAN MANASI</v>
       </c>
       <c r="C78" s="1">
@@ -3323,11 +3323,11 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="str">
-        <f>[1]Sheet1!$A78</f>
+        <f>[2]Sheet1!$A78</f>
         <v>MMS18-20/77</v>
       </c>
       <c r="B79" s="12" t="str">
-        <f>[1]Sheet1!$B78</f>
+        <f>[2]Sheet1!$B78</f>
         <v>PANDYA VANESHA EDWIN SHASHMIRA</v>
       </c>
       <c r="C79" s="1">
@@ -3343,11 +3343,11 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="str">
-        <f>[1]Sheet1!$A79</f>
+        <f>[2]Sheet1!$A79</f>
         <v>MMS18-20/78</v>
       </c>
       <c r="B80" s="12" t="str">
-        <f>[1]Sheet1!$B79</f>
+        <f>[2]Sheet1!$B79</f>
         <v xml:space="preserve">PATEKAR RUPESH GANESH MANJULA </v>
       </c>
       <c r="C80" s="1">
@@ -3363,11 +3363,11 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="str">
-        <f>[1]Sheet1!$A80</f>
+        <f>[2]Sheet1!$A80</f>
         <v>MMS18-20/79</v>
       </c>
       <c r="B81" s="12" t="str">
-        <f>[1]Sheet1!$B80</f>
+        <f>[2]Sheet1!$B80</f>
         <v>PATEL PRAGNESH KISHORBHAI DAMYANTIBEN</v>
       </c>
       <c r="C81" s="1">
@@ -3383,11 +3383,11 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="str">
-        <f>[1]Sheet1!$A81</f>
+        <f>[2]Sheet1!$A81</f>
         <v>MMS18-20/80</v>
       </c>
       <c r="B82" s="12" t="str">
-        <f>[1]Sheet1!$B81</f>
+        <f>[2]Sheet1!$B81</f>
         <v>PATIL CHAITALEE NARESH NAMITA</v>
       </c>
       <c r="C82" s="1">
@@ -3403,11 +3403,11 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="str">
-        <f>[1]Sheet1!$A82</f>
+        <f>[2]Sheet1!$A82</f>
         <v>MMS18-20/81</v>
       </c>
       <c r="B83" s="12" t="str">
-        <f>[1]Sheet1!$B82</f>
+        <f>[2]Sheet1!$B82</f>
         <v>PEDNEKAR MADHUGANDHA DILIP DEEPALI</v>
       </c>
       <c r="C83" s="1">
@@ -3423,11 +3423,11 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="str">
-        <f>[1]Sheet1!$A83</f>
+        <f>[2]Sheet1!$A83</f>
         <v>MMS18-20/82</v>
       </c>
       <c r="B84" s="12" t="str">
-        <f>[1]Sheet1!$B83</f>
+        <f>[2]Sheet1!$B83</f>
         <v>PHANSE SAILEE VINOD LEELA</v>
       </c>
       <c r="C84" s="1">
@@ -3443,11 +3443,11 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="str">
-        <f>[1]Sheet1!$A84</f>
+        <f>[2]Sheet1!$A84</f>
         <v>MMS18-20/83</v>
       </c>
       <c r="B85" s="12" t="str">
-        <f>[1]Sheet1!$B84</f>
+        <f>[2]Sheet1!$B84</f>
         <v>PRASAD ROHAN RAJENDRA RAJKUMARI</v>
       </c>
       <c r="C85" s="1">
@@ -3463,11 +3463,11 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="str">
-        <f>[1]Sheet1!$A85</f>
+        <f>[2]Sheet1!$A85</f>
         <v>MMS18-20/84</v>
       </c>
       <c r="B86" s="12" t="str">
-        <f>[1]Sheet1!$B85</f>
+        <f>[2]Sheet1!$B85</f>
         <v>RAI JAYESH RAVINDRANATH DIVYA</v>
       </c>
       <c r="C86" s="1">
@@ -3483,11 +3483,11 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="str">
-        <f>[1]Sheet1!$A86</f>
+        <f>[2]Sheet1!$A86</f>
         <v>MMS18-20/85</v>
       </c>
       <c r="B87" s="12" t="str">
-        <f>[1]Sheet1!$B86</f>
+        <f>[2]Sheet1!$B86</f>
         <v>RANE ASHWINI SANTOSH SAVITA</v>
       </c>
       <c r="C87" s="1">
@@ -3503,11 +3503,11 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="str">
-        <f>[1]Sheet1!$A87</f>
+        <f>[2]Sheet1!$A87</f>
         <v>MMS18-20/86</v>
       </c>
       <c r="B88" s="12" t="str">
-        <f>[1]Sheet1!$B87</f>
+        <f>[2]Sheet1!$B87</f>
         <v>RANE MAYURI SUHAS ARCHANA</v>
       </c>
       <c r="C88" s="1">
@@ -3523,11 +3523,11 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="str">
-        <f>[1]Sheet1!$A88</f>
+        <f>[2]Sheet1!$A88</f>
         <v>MMS18-20/87</v>
       </c>
       <c r="B89" s="12" t="str">
-        <f>[1]Sheet1!$B88</f>
+        <f>[2]Sheet1!$B88</f>
         <v>RAORANE SAINI SATISH SANCHITA</v>
       </c>
       <c r="C89" s="1">
@@ -3543,11 +3543,11 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="str">
-        <f>[1]Sheet1!$A89</f>
+        <f>[2]Sheet1!$A89</f>
         <v>MMS18-20/88</v>
       </c>
       <c r="B90" s="12" t="str">
-        <f>[1]Sheet1!$B89</f>
+        <f>[2]Sheet1!$B89</f>
         <v>RATHOD OMKAR PANDIT DEVIKA</v>
       </c>
       <c r="C90" s="1">
@@ -3563,11 +3563,11 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="str">
-        <f>[1]Sheet1!$A90</f>
+        <f>[2]Sheet1!$A90</f>
         <v>MMS18-20/89</v>
       </c>
       <c r="B91" s="12" t="str">
-        <f>[1]Sheet1!$B90</f>
+        <f>[2]Sheet1!$B90</f>
         <v>SANGLE SINDHANT NAVANATH PRATIBHA</v>
       </c>
       <c r="C91" s="1">
@@ -3583,11 +3583,11 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="str">
-        <f>[1]Sheet1!$A91</f>
+        <f>[2]Sheet1!$A91</f>
         <v>MMS18-20/90</v>
       </c>
       <c r="B92" s="12" t="str">
-        <f>[1]Sheet1!$B91</f>
+        <f>[2]Sheet1!$B91</f>
         <v>SARMALKAR SANIKA SUNILDATTA MANISHA</v>
       </c>
       <c r="C92" s="1">
@@ -3603,11 +3603,11 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="str">
-        <f>[1]Sheet1!$A92</f>
+        <f>[2]Sheet1!$A92</f>
         <v>MMS18-20/91</v>
       </c>
       <c r="B93" s="12" t="str">
-        <f>[1]Sheet1!$B92</f>
+        <f>[2]Sheet1!$B92</f>
         <v>SATAM NEHA ANIL ASMITA</v>
       </c>
       <c r="C93" s="1">
@@ -3623,11 +3623,11 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="str">
-        <f>[1]Sheet1!$A93</f>
+        <f>[2]Sheet1!$A93</f>
         <v>MMS18-20/92</v>
       </c>
       <c r="B94" s="12" t="str">
-        <f>[1]Sheet1!$B93</f>
+        <f>[2]Sheet1!$B93</f>
         <v>SAWANT AVADHUT RAJAN SHRADDHA</v>
       </c>
       <c r="C94" s="1">
@@ -3643,11 +3643,11 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="str">
-        <f>[1]Sheet1!$A94</f>
+        <f>[2]Sheet1!$A94</f>
         <v>MMS18-20/93</v>
       </c>
       <c r="B95" s="12" t="str">
-        <f>[1]Sheet1!$B94</f>
+        <f>[2]Sheet1!$B94</f>
         <v>SHARMA PALAK PRAHLAD MRIDULA</v>
       </c>
       <c r="C95" s="1">
@@ -3663,11 +3663,11 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="str">
-        <f>[1]Sheet1!$A95</f>
+        <f>[2]Sheet1!$A95</f>
         <v>MMS18-20/94</v>
       </c>
       <c r="B96" s="12" t="str">
-        <f>[1]Sheet1!$B95</f>
+        <f>[2]Sheet1!$B95</f>
         <v>SHETTY SHIFALI PRASHANT ASHALATA</v>
       </c>
       <c r="C96" s="1">
@@ -3683,11 +3683,11 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="str">
-        <f>[1]Sheet1!$A96</f>
+        <f>[2]Sheet1!$A96</f>
         <v>MMS18-20/95</v>
       </c>
       <c r="B97" s="12" t="str">
-        <f>[1]Sheet1!$B96</f>
+        <f>[2]Sheet1!$B96</f>
         <v>SHINDE AKSHAY SURENDRA SUPRIYA</v>
       </c>
       <c r="C97" s="1">
@@ -3703,11 +3703,11 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="str">
-        <f>[1]Sheet1!$A97</f>
+        <f>[2]Sheet1!$A97</f>
         <v>MMS18-20/96</v>
       </c>
       <c r="B98" s="12" t="str">
-        <f>[1]Sheet1!$B97</f>
+        <f>[2]Sheet1!$B97</f>
         <v>SHINDE ASHUTOSH BHASKAR BHAVANA</v>
       </c>
       <c r="C98" s="1">
@@ -3723,11 +3723,11 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="str">
-        <f>[1]Sheet1!$A98</f>
+        <f>[2]Sheet1!$A98</f>
         <v>MMS18-20/97</v>
       </c>
       <c r="B99" s="12" t="str">
-        <f>[1]Sheet1!$B98</f>
+        <f>[2]Sheet1!$B98</f>
         <v>SHINDE NIKHIL KRISHNAT MANISHA</v>
       </c>
       <c r="C99" s="1">
@@ -3743,11 +3743,11 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="str">
-        <f>[1]Sheet1!$A99</f>
+        <f>[2]Sheet1!$A99</f>
         <v>MMS18-20/98</v>
       </c>
       <c r="B100" s="12" t="str">
-        <f>[1]Sheet1!$B99</f>
+        <f>[2]Sheet1!$B99</f>
         <v>SHINDE SAIRAJ VIKAS SHRADHA</v>
       </c>
       <c r="C100" s="1">
@@ -3763,11 +3763,11 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="str">
-        <f>[1]Sheet1!$A100</f>
+        <f>[2]Sheet1!$A100</f>
         <v>MMS18-20/99</v>
       </c>
       <c r="B101" s="12" t="str">
-        <f>[1]Sheet1!$B100</f>
+        <f>[2]Sheet1!$B100</f>
         <v>SHINDE SURAJ SHASHIKANT SHOBHA</v>
       </c>
       <c r="C101" s="1">
@@ -3783,11 +3783,11 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="str">
-        <f>[1]Sheet1!$A101</f>
+        <f>[2]Sheet1!$A101</f>
         <v>MMS18-20/100</v>
       </c>
       <c r="B102" s="12" t="str">
-        <f>[1]Sheet1!$B101</f>
+        <f>[2]Sheet1!$B101</f>
         <v>SHITYALKAR SHUBHAM DHONDIBA SHALAN</v>
       </c>
       <c r="C102" s="1">
@@ -3803,11 +3803,11 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="str">
-        <f>[1]Sheet1!$A102</f>
+        <f>[2]Sheet1!$A102</f>
         <v>MMS18-20/101</v>
       </c>
       <c r="B103" s="12" t="str">
-        <f>[1]Sheet1!$B102</f>
+        <f>[2]Sheet1!$B102</f>
         <v>SHIVKAR PRIYANKA JANARDHAN REKHA</v>
       </c>
       <c r="C103" s="1">
@@ -3823,11 +3823,11 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="str">
-        <f>[1]Sheet1!$A103</f>
+        <f>[2]Sheet1!$A103</f>
         <v>MMS18-20/102</v>
       </c>
       <c r="B104" s="12" t="str">
-        <f>[1]Sheet1!$B103</f>
+        <f>[2]Sheet1!$B103</f>
         <v>SHRIGADI ROHIT DHARMENDRA RUPA</v>
       </c>
       <c r="C104" s="1">
@@ -3843,11 +3843,11 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="str">
-        <f>[1]Sheet1!$A104</f>
+        <f>[2]Sheet1!$A104</f>
         <v>MMS18-20/103</v>
       </c>
       <c r="B105" s="12" t="str">
-        <f>[1]Sheet1!$B104</f>
+        <f>[2]Sheet1!$B104</f>
         <v>SINGH PRATIK SANJAY MEENA</v>
       </c>
       <c r="C105" s="1">
@@ -3863,11 +3863,11 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="str">
-        <f>[1]Sheet1!$A105</f>
+        <f>[2]Sheet1!$A105</f>
         <v>MMS18-20/104</v>
       </c>
       <c r="B106" s="12" t="str">
-        <f>[1]Sheet1!$B105</f>
+        <f>[2]Sheet1!$B105</f>
         <v>SINGH VARSHA GURUPRASAD VEENA</v>
       </c>
       <c r="C106" s="1">
@@ -3883,11 +3883,11 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="str">
-        <f>[1]Sheet1!$A106</f>
+        <f>[2]Sheet1!$A106</f>
         <v>MMS18-20/105</v>
       </c>
       <c r="B107" s="12" t="str">
-        <f>[1]Sheet1!$B106</f>
+        <f>[2]Sheet1!$B106</f>
         <v>SOLANKI PRAKASH RAMESH SUREKHA</v>
       </c>
       <c r="C107" s="1">
@@ -3903,11 +3903,11 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="str">
-        <f>[1]Sheet1!$A107</f>
+        <f>[2]Sheet1!$A107</f>
         <v>MMS18-20/106</v>
       </c>
       <c r="B108" s="12" t="str">
-        <f>[1]Sheet1!$B107</f>
+        <f>[2]Sheet1!$B107</f>
         <v>SURYAVANSHI MAYURI DILIP BHAGIRATHI</v>
       </c>
       <c r="C108" s="1">
@@ -3923,11 +3923,11 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="str">
-        <f>[1]Sheet1!$A108</f>
+        <f>[2]Sheet1!$A108</f>
         <v>MMS18-20/107</v>
       </c>
       <c r="B109" s="12" t="str">
-        <f>[1]Sheet1!$B108</f>
+        <f>[2]Sheet1!$B108</f>
         <v>SWAMY VIOLET BENEDICT JULIET</v>
       </c>
       <c r="C109" s="1">
@@ -3943,11 +3943,11 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="str">
-        <f>[1]Sheet1!$A109</f>
+        <f>[2]Sheet1!$A109</f>
         <v>MMS18-20/108</v>
       </c>
       <c r="B110" s="12" t="str">
-        <f>[1]Sheet1!$B109</f>
+        <f>[2]Sheet1!$B109</f>
         <v xml:space="preserve">TAKKE SAIRAJ SURESH SHRUTIKA </v>
       </c>
       <c r="C110" s="1">
@@ -3963,11 +3963,11 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="str">
-        <f>[1]Sheet1!$A110</f>
+        <f>[2]Sheet1!$A110</f>
         <v>MMS18-20/109</v>
       </c>
       <c r="B111" s="12" t="str">
-        <f>[1]Sheet1!$B110</f>
+        <f>[2]Sheet1!$B110</f>
         <v>TALELE BHOOMA GHANASHYAM KALPANA</v>
       </c>
       <c r="C111" s="1">
@@ -3983,11 +3983,11 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="str">
-        <f>[1]Sheet1!$A111</f>
+        <f>[2]Sheet1!$A111</f>
         <v>MMS18-20/110</v>
       </c>
       <c r="B112" s="12" t="str">
-        <f>[1]Sheet1!$B111</f>
+        <f>[2]Sheet1!$B111</f>
         <v>THOOLKAR SAMEER ARVIND KIRAN</v>
       </c>
       <c r="C112" s="1">
@@ -4003,11 +4003,11 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="str">
-        <f>[1]Sheet1!$A112</f>
+        <f>[2]Sheet1!$A112</f>
         <v>MMS18-20/111</v>
       </c>
       <c r="B113" s="12" t="str">
-        <f>[1]Sheet1!$B112</f>
+        <f>[2]Sheet1!$B112</f>
         <v>TIWARI VIKAS CHINTAMANI SHAILA</v>
       </c>
       <c r="C113" s="1">
@@ -4023,11 +4023,11 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="str">
-        <f>[1]Sheet1!$A113</f>
+        <f>[2]Sheet1!$A113</f>
         <v>MMS18-20/112</v>
       </c>
       <c r="B114" s="12" t="str">
-        <f>[1]Sheet1!$B113</f>
+        <f>[2]Sheet1!$B113</f>
         <v>TREHAN VILAKSHAN SUMAN NEENA</v>
       </c>
       <c r="C114" s="1">
@@ -4043,11 +4043,11 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="str">
-        <f>[1]Sheet1!$A114</f>
+        <f>[2]Sheet1!$A114</f>
         <v>MMS18-20/113</v>
       </c>
       <c r="B115" s="12" t="str">
-        <f>[1]Sheet1!$B114</f>
+        <f>[2]Sheet1!$B114</f>
         <v>VHAVALE YOGESH VIJANAND ANITA</v>
       </c>
       <c r="C115" s="1">
@@ -4063,11 +4063,11 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="str">
-        <f>[1]Sheet1!$A115</f>
+        <f>[2]Sheet1!$A115</f>
         <v>MMS18-20/114</v>
       </c>
       <c r="B116" s="12" t="str">
-        <f>[1]Sheet1!$B115</f>
+        <f>[2]Sheet1!$B115</f>
         <v>VICHARE SAMRUDHI SANJAY VAIBHAVI</v>
       </c>
       <c r="C116" s="1">
@@ -4083,11 +4083,11 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="str">
-        <f>[1]Sheet1!$A116</f>
+        <f>[2]Sheet1!$A116</f>
         <v>MMS18-20/115</v>
       </c>
       <c r="B117" s="12" t="str">
-        <f>[1]Sheet1!$B116</f>
+        <f>[2]Sheet1!$B116</f>
         <v>WAGHMARE SHEETAL SURYAKANT SUNANDA</v>
       </c>
       <c r="C117" s="1">
@@ -4103,11 +4103,11 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="str">
-        <f>[1]Sheet1!$A117</f>
+        <f>[2]Sheet1!$A117</f>
         <v>MMS18-20/116</v>
       </c>
       <c r="B118" s="12" t="str">
-        <f>[1]Sheet1!$B117</f>
+        <f>[2]Sheet1!$B117</f>
         <v>WANI SHUBHAM RAJENDRA  JYOTI</v>
       </c>
       <c r="C118" s="1">
@@ -4123,11 +4123,11 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="str">
-        <f>[1]Sheet1!$A118</f>
+        <f>[2]Sheet1!$A118</f>
         <v>MMS18-20/117</v>
       </c>
       <c r="B119" s="12" t="str">
-        <f>[1]Sheet1!$B118</f>
+        <f>[2]Sheet1!$B118</f>
         <v>YADAV ANKITA OMPRAKASH SHASHANK DEVI</v>
       </c>
       <c r="C119" s="1">
@@ -4143,11 +4143,11 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="str">
-        <f>[1]Sheet1!$A119</f>
+        <f>[2]Sheet1!$A119</f>
         <v>MMS18-20/118</v>
       </c>
       <c r="B120" s="12" t="str">
-        <f>[1]Sheet1!$B119</f>
+        <f>[2]Sheet1!$B119</f>
         <v>YADAV ANUSH MAHANTA MALTI</v>
       </c>
       <c r="C120" s="1">
@@ -4163,11 +4163,11 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="str">
-        <f>[1]Sheet1!$A120</f>
+        <f>[2]Sheet1!$A120</f>
         <v>MMS18-20/119</v>
       </c>
       <c r="B121" s="12" t="str">
-        <f>[1]Sheet1!$B120</f>
+        <f>[2]Sheet1!$B120</f>
         <v>YADAV SUMAN RAMJEET SAVITRIDEVI</v>
       </c>
       <c r="C121" s="1">
@@ -4183,11 +4183,11 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="str">
-        <f>[1]Sheet1!$A121</f>
+        <f>[2]Sheet1!$A121</f>
         <v>MMS18-20/120</v>
       </c>
       <c r="B122" s="12" t="str">
-        <f>[1]Sheet1!$B121</f>
+        <f>[2]Sheet1!$B121</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C122" s="1">
@@ -4203,11 +4203,11 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="str">
-        <f>[1]Sheet1!$A122</f>
+        <f>[2]Sheet1!$A122</f>
         <v>MMS18-20/121</v>
       </c>
       <c r="B123" s="12" t="str">
-        <f>[1]Sheet1!$B122</f>
+        <f>[2]Sheet1!$B122</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C123" s="1">
@@ -4223,11 +4223,11 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="str">
-        <f>[1]Sheet1!$A123</f>
+        <f>[2]Sheet1!$A123</f>
         <v>MMS18-20/122</v>
       </c>
       <c r="B124" s="12" t="str">
-        <f>[1]Sheet1!$B123</f>
+        <f>[2]Sheet1!$B123</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C124" s="1">
@@ -4243,11 +4243,11 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="str">
-        <f>[1]Sheet1!$A124</f>
+        <f>[2]Sheet1!$A124</f>
         <v>MMS18-20/123</v>
       </c>
       <c r="B125" s="12" t="str">
-        <f>[1]Sheet1!$B124</f>
+        <f>[2]Sheet1!$B124</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C125" s="1">
@@ -4263,11 +4263,11 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="str">
-        <f>[1]Sheet1!$A125</f>
+        <f>[2]Sheet1!$A125</f>
         <v>MMS18-20/124</v>
       </c>
       <c r="B126" s="12" t="str">
-        <f>[1]Sheet1!$B125</f>
+        <f>[2]Sheet1!$B125</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C126" s="1">
@@ -4283,11 +4283,11 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="str">
-        <f>[1]Sheet1!$A126</f>
+        <f>[2]Sheet1!$A126</f>
         <v>MMS18-20/125</v>
       </c>
       <c r="B127" s="12" t="str">
-        <f>[1]Sheet1!$B126</f>
+        <f>[2]Sheet1!$B126</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C127" s="1">
@@ -4303,11 +4303,11 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="str">
-        <f>[1]Sheet1!$A127</f>
+        <f>[2]Sheet1!$A127</f>
         <v>MMS18-20/126</v>
       </c>
       <c r="B128" s="12" t="str">
-        <f>[1]Sheet1!$B127</f>
+        <f>[2]Sheet1!$B127</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C128" s="1">
@@ -4323,11 +4323,11 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="str">
-        <f>[1]Sheet1!$A128</f>
+        <f>[2]Sheet1!$A128</f>
         <v>MMS18-20/127</v>
       </c>
       <c r="B129" s="12" t="str">
-        <f>[1]Sheet1!$B128</f>
+        <f>[2]Sheet1!$B128</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C129" s="1">
@@ -4343,11 +4343,11 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="str">
-        <f>[1]Sheet1!$A129</f>
+        <f>[2]Sheet1!$A129</f>
         <v>MMS18-20/128</v>
       </c>
       <c r="B130" s="12" t="str">
-        <f>[1]Sheet1!$B129</f>
+        <f>[2]Sheet1!$B129</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C130" s="1">
@@ -4363,11 +4363,11 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="str">
-        <f>[1]Sheet1!$A130</f>
+        <f>[2]Sheet1!$A130</f>
         <v>MMS18-20/129</v>
       </c>
       <c r="B131" s="12" t="str">
-        <f>[1]Sheet1!$B130</f>
+        <f>[2]Sheet1!$B130</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C131" s="1">
@@ -4383,11 +4383,11 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="str">
-        <f>[1]Sheet1!$A131</f>
+        <f>[2]Sheet1!$A131</f>
         <v>MMS18-20/130</v>
       </c>
       <c r="B132" s="12" t="str">
-        <f>[1]Sheet1!$B131</f>
+        <f>[2]Sheet1!$B131</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C132" s="1">
@@ -4403,11 +4403,11 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="str">
-        <f>[1]Sheet1!$A132</f>
+        <f>[2]Sheet1!$A132</f>
         <v>MMS18-20/131</v>
       </c>
       <c r="B133" s="12" t="str">
-        <f>[1]Sheet1!$B132</f>
+        <f>[2]Sheet1!$B132</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C133" s="1">
@@ -4423,11 +4423,11 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="str">
-        <f>[1]Sheet1!$A133</f>
+        <f>[2]Sheet1!$A133</f>
         <v>MMS18-20/132</v>
       </c>
       <c r="B134" s="12" t="str">
-        <f>[1]Sheet1!$B133</f>
+        <f>[2]Sheet1!$B133</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C134" s="1">
@@ -4443,11 +4443,11 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="str">
-        <f>[1]Sheet1!$A134</f>
+        <f>[2]Sheet1!$A134</f>
         <v>MMS18-20/133</v>
       </c>
       <c r="B135" s="12" t="str">
-        <f>[1]Sheet1!$B134</f>
+        <f>[2]Sheet1!$B134</f>
         <v>*** (NOT AVAILABLE) ***</v>
       </c>
       <c r="C135" s="1">
@@ -4462,7 +4462,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jTK+fhSNcsxv0rU1Ypgcl1BGw24tFhmTu5DxV5HSTvyAp9iGoKURpxzZ7r+AsY7NVrxOu+ObB0iHvoDr9v+WUg==" saltValue="ARhjell/YDFJ3YLj66eZQw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ICYHL6qPh6waQFxMbxND0lkiMMUu+25duxZPZ8yGLRR6wxqpLPfjdp3Oj7Vk3Rkl0lHBtal20KUuhyoigbU+bQ==" saltValue="TVPlXcZv/MLnsJcm5dSekQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="C3:D135" name="Abhishek"/>
   </protectedRanges>

</xml_diff>